<commit_message>
feat - Melhorando código principal - funcionamento por json
</commit_message>
<xml_diff>
--- a/Vagas-Catho.xlsx
+++ b/Vagas-Catho.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>vaga</t>
+          <t>localizacao</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>link vaga</t>
         </is>
       </c>
     </row>
@@ -466,43 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DNA Cury Júnior | Programa Jovem Aprendiz- Projeto Executivo RJ</t>
+          <t>Vaga de Estágio em Pedagogia</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cury Construtora</t>
+          <t>FADELITO GLOBAL</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-Quem Somos?
- Você sabia que estamos entre as 10 maiores construtoras do país e que atualmente ocupamos o ranking das 150 empresas do novo mercado?
-Estamos na bolsa de valores e temos mais de 2 mil Profissionais Cury que diariamente são movidos pelo desafio de realizar o sonho de milhões de brasileiros: a aquisição da casa própria.
-Somos apaixonados pelo que fazemos, seja na cadeia produtiva ou na comercialização dos empreendimentos.
- Gostou? Prazer, somos a Cury, venha fazer parte da nossa história!
- Conheça as nossas etapas do processo seletivo:
-·        Inscrição em nossa plataforma e seleção dos currículos
-·        Análise dos testes de acordo com o perfil da vaga
-·        Bate-papo com o time de R&amp;S
-·        Bate-papo com o Gestor da vaga
-·        Feedback da sua candidatura
-Obs: essas etapas podem sofrer alterações de acordo com a necessidade da vaga.
- Ah... pessoas com deficiências são super bem-vindas viu?
- Acredita que não preenche todos os requisitos?
- Um estudo recente do LinkedIn indicou que mulheres são menos propensas a se candidatarem a vagas se não acreditarem que preenchem 100% das qualificações. Em comparação, homens tendem a se inscrever mesmo atendendo 60%. Aqui na Cury, queremos construir um ambiente de trabalho cada vez mais diversos e inclusivo. Abaixo estão listadas as responsabilidades e atribuições para posição, porém, se você acredita que sua experiência prévia não se alinha exatamente com todos os pré-requisitos, te incentivamos a se candidatar de qualquer maneira caso tenha se identificado com a posição. Você pode ser a pessoa certa e não queremos perder a chance de te conhecer.
- Você curtiu? Estamos aguardando a sua candidatura!</t>
+          <t>Auxiliar na elaboração de planos de aula Apoiar na execução de atividades pedagógica Acompanhar o desenvolvimento dos alunos Colaborar na organização de eventos educacionais Contribuir para a melhoria contínua dos processos educacionais</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Até R$ 2.000,00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP (1)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30447734/</t>
         </is>
       </c>
     </row>
@@ -512,43 +506,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DNA Cury Júnior | Programa Jovem Aprendiz Obra Americas 19 ( Helbor ) RJ</t>
+          <t>Vaga de Estágio</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Cury Construtora</t>
+          <t>EMPRESA CONFIDENCIAL</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-Quem Somos?
- Você sabia que estamos entre as 10 maiores construtoras do país e que atualmente ocupamos o ranking das 150 empresas do novo mercado?
-Estamos na bolsa de valores e temos mais de 2 mil Profissionais Cury que diariamente são movidos pelo desafio de realizar o sonho de milhões de brasileiros: a aquisição da casa própria.
-Somos apaixonados pelo que fazemos, seja na cadeia produtiva ou na comercialização dos empreendimentos.
- Gostou? Prazer, somos a Cury, venha fazer parte da nossa história!
- Conheça as nossas etapas do processo seletivo:
-·        Inscrição em nossa plataforma e seleção dos currículos
-·        Análise dos testes de acordo com o perfil da vaga
-·        Bate-papo com o time de R&amp;S
-·        Bate-papo com o Gestor da vaga
-·        Feedback da sua candidatura
-Obs: essas etapas podem sofrer alterações de acordo com a necessidade da vaga.
- Ah... pessoas com deficiências são super bem-vindas viu?
- Acredita que não preenche todos os requisitos?
- Um estudo recente do LinkedIn indicou que mulheres são menos propensas a se candidatarem a vagas se não acreditarem que preenchem 100% das qualificações. Em comparação, homens tendem a se inscrever mesmo atendendo 60%. Aqui na Cury, queremos construir um ambiente de trabalho cada vez mais diversos e inclusivo. Abaixo estão listadas as responsabilidades e atribuições para posição, porém, se você acredita que sua experiência prévia não se alinha exatamente com todos os pré-requisitos, te incentivamos a se candidatar de qualquer maneira caso tenha se identificado com a posição. Você pode ser a pessoa certa e não queremos perder a chance de te conhecer.
- Você curtiu? Estamos aguardando a sua candidatura!</t>
+          <t>Realizar atendimentos aos pacientes na recepção
+Realizar agendamentos via WhatsApp
+Auxiliar nas atividades administrativas da clínica
+Colaborar com a equipe multidisciplinar Boa comunicação</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Até R$ 2.000,00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>Sorocaba - SP (1)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio/30702202/</t>
         </is>
       </c>
     </row>
@@ -558,32 +544,38 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Analista de Marketing Junior- Programa de Benefícios- Shopping Plaza Sul</t>
+          <t>Vaga de Estágio</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cury Construtora</t>
+          <t>EMPRESA CONFIDENCIAL</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-ALLOS é uma marca com uma forte herança. São cerca de 50 anos de experiência, transformando o mercado no Brasil. Somos referência em excelência e inovação, com a qualidade e confiança que faz parte da nossa história.
- A nova marca surgiu pronta para o futuro, a partir da fusão entre a Aliansce Sonae e a brMalls, em 2023. Mas, essa trajetória começou bem antes.
- Tudo começou com a Aliansce, que inaugurou o primeiro shopping da região Nordeste e o segundo do Brasil em 1975. Em 2019, a fusão entre a Aliansce e a Sonae Sierra deu origem à Aliansce Sonae, tornando-se líder na administração de shoppings no Brasil, com 32 empreendimentos. Em 2006, surge a brMalls resultando em um portfólio de 30 ativos presentes nas cinco regiões do país.
- E assim, em 2023, a ALLOS surge com o encontro de duas potências nacionais do segmento, unindo forças para se tornar a mais inovadora plataforma de entretenimento, lifestyle, serviços e compras.
-Nossa história continua e estamos prontos para criar momentos que transformam e impactam a vida das pessoas, gerando conexões e oportunidades.</t>
+          <t>Auxiliar na separação de peças conferencia dos pedidos etiquetar produtos organizar locação de peças 
+ Cursando ensino superior em Engenharia Elétrica Mecânica ou áreas afins
+Conhecimento básico em componentes automotivos
+Boa comunicação e habilidades interpessoais
+Experiência prévia em estágios na área automotiv
+Conhecimento em sistemas de gestão
+Inglês intermediário</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A combinar</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Caxias do Sul - RS (1)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio/30703859/</t>
         </is>
       </c>
     </row>
@@ -593,32 +585,33 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Programador Junior</t>
+          <t>Vaga de Estágio</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cury Construtora</t>
+          <t>EMPRESA CONFIDENCIAL</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-Temos a missão de facilitar o dia a dia das pessoas através dos nossos softwares para diferentes segmentos do mercado. Para isso acontecer, contamos com um time incrível, composto por pessoas apaixonadas e engajadas em um único propósito: oferecer ferramentas inovadoras.
- Nosso convite é pensar juntos para melhorar o que existe, e ir além!
- Esse pode ser seu novo desafio para aprender, crescer, transformar e inovar, com a oportunidade de desenvolver sua carreira em uma das principais empresas de software do Brasil.
-Venha fazer parte dessa empresa incrível!
-Seja um Benner!</t>
+          <t>Recebimento de Mercadoria Conferência e Embalagem de Produtos Contagem cíclica de estoques Expedição de Pedidos Conferência de Nota Fiscal recebida Reposição de Estoques Separação de Pedidos Organizado responsável proativo ágil
+Requisitos técnicos Conhecimento World Excel</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A combinar</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Caxias do Sul - RS (1)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio/30702704/</t>
         </is>
       </c>
     </row>
@@ -628,30 +621,41 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Programa Gerente Júnior Business (Joinville/SC)</t>
+          <t>Vaga de estágio</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Cury Construtora</t>
+          <t>LUIZ EDMUNDO MACHADO CORRETAGEM DE IMOVEIS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-Nossa gente aqui na Cervejaria Ambev sonha GRANDE! Somos milhares de apaixonados pelo que fazemos. Nosso maior objetivo é inovar no setor de bebidas com a maior qualidade e diversidade possível, para que você possa brindar qualquer ocasião escolhendo o que mais gosta!
-A nossa Cultura é focada em construir um ambiente inclusivo e colaborativo, onde as pessoas possam ser o melhor delas mesmas! Gente é o nosso maior ativo, afinal sabemos que investir no potencial de nossos colaboradores é trazer ainda mais qualidade ao nosso negócio e às nossas bebidas. Por isso, estamos sempre em busca de talentos diversos, dispostos a construir esse grande sonho com a gente de unir as pessoas por um mundo melhor.
-Prazer, somos a Cervejaria Ambev e adoraríamos te ter com a gente.</t>
+          <t>Auxiliar no atendimento aos clientes e na prospecção de novos negócios
+Realizar visitas a imóveis e apresentar as opções disponíveis
+Participar de reuniões e treinamentos para aprimorar conhecimentos
+Manter atualizado o sistema de cadastro de imóveis
+Auxiliar na elaboração de contratos de compra e venda
+Colaborar com a equipe em atividades administrativas Ensino Médio completo
+Conhecimento básico em informática
+Boa comunicação oral e escrita
+Experiência prévia em atendimento ao cliente
+Espirito empreendedor</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Até R$ 2.000,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>São Paulo - SP (1)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio/30681882/</t>
         </is>
       </c>
     </row>
@@ -661,30 +665,766 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PROGRAMADOR RPA JUNIOR</t>
+          <t>Vaga de estágio</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cury Construtora</t>
+          <t>CLÍNICA LIFE FISIO SANTOS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Acompanhar a Fisioterapeuta em sessões de fisioterapia ortopédica ou desportiva
+Aplicar Aula de Pilates junto com a fisioterapeuta
+Aplicar quando necessário liberação miofascial e drenagem linfática Curso de Pilates</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Santos - SP (2)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio/30675494/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio Direito</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>PERIM AUTO PEÇAS</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Elaboração de peça processual 1º e 2º grau
+Acompanhamento de processos
+Emissão de Guias
+Relatórios 
+Negociação Judicial e Extrajudicial
+Pesquisa Jurisprudencial
+Controle de Prazos</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Até R$ 2.000,00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>São Paulo - SP (1)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-direito/30701381/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio em Pedagogia</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>AGIEER</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ATIVIDADES Assistirá e acompanhará na recepção das criançasfamília e colher informações sobre a criança na entrada bem como repassar informações sobre a criança na saída auxiliar na análise e solicitar à família reposição de materiais de higiene pessoal da criança auxiliar no banho e troca das crianças e realizar os cuidados no despertar das crianças dar suporte ao lactário nas informações sobre a criança para a distribuição individual dos alimentos e bebidas ajudar no oferecimento à criança contribuir com informações para preenchimento de relatórios com as informações das crianças referentes a alimentação trocas de fralda sinais e sintomas elaborar registros de atividades participar de reuniões participar de treinamentos auxiliar na organização e do parque na confecção de materiais de eventos e brinquedos educativos auxiliar nos ensinamentos e nos cuidados e devoluções dos utensílios utilizados nas alimentações reposição de material de higiene e consumo organizar brinquedos pós higienização controlar e cuidas das trocas de roupas de cama REQUISITOS Residir na região da Lapa ou proximidades e estar cursando Pedagogia</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Até R$ 2.000,00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>São Paulo - SP (1)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30701138/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Vaga de ESTÁGIO ADMINISTRATIVO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>OUTLET DA CONSTRUÇÃO LTDA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Auxiliar no cadastro de fornecedores e produtos Apoiar autorizando notas de compras no sistema Apoiar em lançamentos de notas fiscais Auxiliar no controle das notas faturadas no CNPJ da empresa Auxiliar na emissão de notas de devolução de fornecedores baixas e transferência de estoque e bonificações Auxiliar no controle de estoque dos produtos emissão de nota de baixaentrada dos mesmos A partir do 3º período CIÊNCIAS CONTÁBEIS Segunda a Sexta 08h as 12h e das 13h as 15h com 1h de almoço Valor da bolsa R100000 e vale transporte</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Até R$ 2.000,00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Lauro de Freitas - BA (1)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-administrativo/30700649/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Vaga de ESTÁGIO EM PEDAGOGIA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>EMPRESA CONFIDENCIAL</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Seu currículo foi selecionado em nosso banco de dados para participar de um processo seletivo conforme condições abaixo
+Vaga Estágio Pedagogia
+Regime Contrato 6 meses
+Bolsa Auxílio R 85000
+Benefícios Vale transporte cesta básica possibilidade de prorrogação e possibilidade de efetivação
+Quantidade de vagas 2
+Horário do Estágio Das 1100 hs às 1700 hs
+Início Imediato
+Requisitos Pontualidade organização e atuação com qualidade e compromisso nos procedimentos estabelecidos no regimento escolar
+Nível Superior em Pedagogia  cursando 
+Horário de estudo A distância Noturno
+Atividades de estágio auxiliar no desenvolvimento de atividades pedagógicas prestar apoio na elaboração de projetos educacionais desenvolver atividades recreativas assessorar a professora nas rotinas de cuidados em sala de aula higiene alimenteção etc Até 4º Semestre</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Até R$ 2.000,00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Ribeirão Pires - SP (2)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30054732/</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Vaga de Estagio em Direito</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ROCHA MARINHO E SALES ADVOGADOS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Acompanhar audiências judiciais representando o escritório em casos de menor complexidade sob a supervisão de advogados
+Elaborar atas minutas de audiências e pareceres processuais
+Preparar e organizar documentos a serem utilizados nas audiências
+Realizar diligências externas junto aos fóruns e tribunais
+Prestar suporte aos advogados auxiliando na análise e no acompanhamento de processos</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Até R$ 2.000,00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Fortaleza - CE (1)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-direito/30702103/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio de Direito</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>EMPRESA CONFIDENCIAL</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Protocolos Guias Organização de arquivos Petições diversas Andamento processual Atendimento ao cliente Perfil analítico Comprometimento Próatividade Organização Pontualidade Pacote office Excelente comunicação verbal e escrita Deve ter experiências em escritórios de advocacia Residir em CampinasSP</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Campinas - SP (1)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-de-direito/30700977/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio em Administração</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SAMVARDHANA MOTHERSON REYDEL COMPANIES</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>A Motherson Group é um fornecedor de soluções completas para a indústria automotiva global está entre os 21 maiores fornecedores com mais rápido crescimento atende a várias indústrias tais como material rodante aeroespacial médico TI e logística com mais de 135000 colaboradores mundialmente distribuídos em 42 países pelo mundo 
+Samvardhana Motherson Reydel Companies SMRC é a especialista do grupo em interiores inovadores de automóveis e caminhões Com instalações na Europa Ásia e América do Sul projetamos desenvolvemos e fabricamos sistemas internos completos de alta qualidade como cockpits consoles centrais painéis de portas e superfícies decorativas para várias montadoras de veículos em todo o mundo Em razão do nosso rápido crescimento estamos constantemente procurando novos e talentosos colegas para fazerem parte da nossa equipe
+Você está procurando uma oportunidade de crescimento e desenvolvimento na área de Administração
+A Motherson Group uma grande empresa do setor automotivo está com uma vaga de Estágio em Administração disponível
+Como estagiárioa de Administração você será responsável por
+ Auxiliar nas atividades administrativas da empresa como controle de documentos arquivamento atendimento ao público e organização de rotinas
+ Participar de projetos e atividades relacionadas à área de Administração como análise de processos elaboração de relatórios e suporte a tomada de decisões
+ Aprender e adquirir novas habilidades aplicando os conhecimentos adquiridos durante sua formação acadêmica   Para se candidatar a esta vaga é necessário
+ Estar cursando Administração ou áreas afins formação a partir de 2026
+ Possuir habilidades de comunicação organização e trabalho em equipe
+ Ter conhecimentos básicos em informática como pacote Office
+ Ser proativoa comprometidoa e interessadoa em aprender</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>São Paulo - SP (1)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-administracao/30701178/</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio em Nutrição</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>B&amp;P DESENVOLVIMENTO HUMANO</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Auxiliar na elaboração e controle de cardápios e fichas técnicas de produção considerando aspectos nutricionais e legislações vigentes
+  Acompanhar a implementação das boas práticas de manipulação de alimentos BPF e do controle de qualidade
+  Apoiar a equipe na verificação de validade e condições de armazenamento dos insumos alimentares
+  Colaborar na realização de treinamentos sobre higiene segurança alimentar e manipulação de alimentos para a equipe da padaria
+  Participar do controle de custos ajudando na gestão de desperdícios e na otimização de ingredientes
+  Monitorar o atendimento a requisitos de dietas especiais como opções sem glúten ou lactose
+  Auxiliar no desenvolvimento de novos produtos e receitas nutritivas para o portfólio da padaria
+   Cursando Técnico ou Superior em Nutrição
+ </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Santo Andre - SP (1)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-nutricao/30701246/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio de Direito</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ROSSI ADVOCACIA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Guias Organização de arquivos Petições diversas Andamento processual Atendimento ao cliente protocolos Cursando Direito Perfil analítico Comprometimento Próatividade Organização Pontualidade Pacote office Excelente comunicação verbal e escrita Deve ter experiências em escritórios de advocacia Residir em CampinasSP</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Campinas - SP (1)</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-de-direito/30700940/</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio em Direito</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>OLÍMPIO DE AZEVEDO ADVOGADOS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Estágio em Direito Interno  Auxiliar o Advogado em consulta processual aos principais sites do judiciário  Elaboração e conferência de guias de recolhimento de custas judiciais  Complementação de cadastros  Peticionamento simples em conjunto com o Advogado  Preenchimento de planilhas relatórios  Digitalização e arquivamento de documentos e correspondências jurídicas  Obtenção de cópias  Carga de processos  Despacho de petições com juízes Benefícios Seguro de Vida em Grupo Vale Transporte Regime de contratação Estágio Horário A combinar Deverá estar cursando Ensino Superior em Direito Pacote office básico Vontade de aprender</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>São Paulo - SP (1)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://www.catho.com.br/vagas/estagio-em-direito/30701062/</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>4016474 : Programa de Estágio TIM RJ</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4016474 : Programa de Estágio TIM RJ</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>DESCRIÇÃO DA VAGA
-Se você é um profissional analítico, organizado, com senso de prioridades e tem facilidade de trabalhar em equipe, essa é a oportunidade de agregar em nosso time.
-Um dos grandes princípios da S. Magalhães &amp; Essemaga é dar a cada colaborador(a) a oportunidade de desenvolver o seu potencial em um ambiente de trabalho seguro e justo, onde as pessoas possam ser ouvidas, respeitadas e valorizadas. Queremos junto a você chegar ainda mais longe em nossa caminhada!
-Venha fazer parte da equipe S. Magalhães &amp; Essemaga.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Santos - SP</t>
+SomosMaisNaTIM Fazer parte da TIM é se conectar com o que acreditamos e ter MAIS sintonia com todo o TIMe É aprender novas formas de oferecer ao mundo um trabalho com MAIS propósito Aprendizado na TIM é MAIS que possibilidade É o que nos move a fazer MAIS e melhor É desenvolver habilidades com criatividade e transformar tecnologia em MAIS liberdade Tecnologia na TIM é MAIS que ter a melhor cobertura É imaginar as possibilidades com MAIS inovação conectando todos e todas com respeito e agilidade Diversidade e Inclusão na TIM é MAIS que abraçar É uma cultura cada vez MAIS essencial para o nosso dia a dia É criar um impacto MAIS positivo sendo quem você é Vem ser você e fazer parte de um TIMe que tem a coragem para inovar a liberdade para tentar e a vontade de fazer a diferença na vida das pessoas imagineaspossibilidades</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://programastim.gupy.io/job/eyJqb2JJZCI6Nzk5ODg0OCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4013980 : Programa de Estágio TIM RJ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4013980 : Programa de Estágio TIM RJ</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+SomosMaisNaTIM Fazer parte da TIM é se conectar com o que acreditamos e ter MAIS sintonia com todo o TIMe É aprender novas formas de oferecer ao mundo um trabalho com MAIS propósito Aprendizado na TIM é MAIS que possibilidade É o que nos move a fazer MAIS e melhor É desenvolver habilidades com criatividade e transformar tecnologia em MAIS liberdade Tecnologia na TIM é MAIS que ter a melhor cobertura É imaginar as possibilidades com MAIS inovação conectando todos e todas com respeito e agilidade Diversidade e Inclusão na TIM é MAIS que abraçar É uma cultura cada vez MAIS essencial para o nosso dia a dia É criar um impacto MAIS positivo sendo quem você é Vem ser você e fazer parte de um TIMe que tem a coragem para inovar a liberdade para tentar e a vontade de fazer a diferença na vida das pessoas imagineaspossibilidades</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://programastim.gupy.io/job/eyJqb2JJZCI6Nzk5ODgwMCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PROGRAMA DE ESTÁGIO 2025 - FARMÁCIA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>PROGRAMA DE ESTÁGIO 2025 - FARMÁCIA</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+Estão abertas as inscrições para o Programa de Estágio em Farmácia 2025 do Hospital Alemão Oswaldo Cruz
+Venha fazer parte de um time que é referência no País responsável por colaborar e destacar o Oswaldo Cruz como um dos melhores centros hospitalares da América Latina
+O Hospital é composto por pessoas que têm compromisso com o paciente e foco em qualidade e segurança Somos orientados para o resultado e por isso temos uma atuação inovadora e liderança inspiradora Estamos há 126 anos promovendo o cuidado inclusive de quem cuida
+Trazemos de nossa origem alemã algumas características como o respeito pelo outro a valorização do coletivo a verdade a discrição e a austeridade E isso se reflete ao que todos os colaboradores se propõem a cada dia Immer Besser  Fazer sempre melhor</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>São Paulo - SP</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://hospitaloswaldocruz.gupy.io/job/eyJqb2JJZCI6Nzk5ODI5MSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>4045902 : Programa de Estágio TIM RJ</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>4045902 : Programa de Estágio TIM RJ</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+SomosMaisNaTIM Fazer parte da TIM é se conectar com o que acreditamos e ter MAIS sintonia com todo o TIMe É aprender novas formas de oferecer ao mundo um trabalho com MAIS propósito Aprendizado na TIM é MAIS que possibilidade É o que nos move a fazer MAIS e melhor É desenvolver habilidades com criatividade e transformar tecnologia em MAIS liberdade Tecnologia na TIM é MAIS que ter a melhor cobertura É imaginar as possibilidades com MAIS inovação conectando todos e todas com respeito e agilidade Diversidade e Inclusão na TIM é MAIS que abraçar É uma cultura cada vez MAIS essencial para o nosso dia a dia É criar um impacto MAIS positivo sendo quem você é Vem ser você e fazer parte de um TIMe que tem a coragem para inovar a liberdade para tentar e a vontade de fazer a diferença na vida das pessoas imagineaspossibilidades</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://programastim.gupy.io/job/eyJqb2JJZCI6Nzk5NzIzNiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Estágio Jurídico</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Estágio Jurídico</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais arbitrais e extrajudiciais
+Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias pareceres opiniões legais desenvolvimento de negócios elaboração e estruturação de contratos
+O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito seja no âmbito regional nacional ou internacional São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Campo Grande - MS</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6Nzk5ODE5NSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Estágio Jurídico</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Estágio Jurídico</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais arbitrais e extrajudiciais
+Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias pareceres opiniões legais desenvolvimento de negócios elaboração e estruturação de contratos
+O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito seja no âmbito regional nacional ou internacional São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Campo Grande - MS</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6Nzk5ODE4Nywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Estágio Jurídico</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Estágio Jurídico</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais arbitrais e extrajudiciais
+Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias pareceres opiniões legais desenvolvimento de negócios elaboração e estruturação de contratos
+O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito seja no âmbito regional nacional ou internacional São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Campo Grande - MS</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6Nzk5ODE4Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Estagiária(o) Superior</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Estagiária(o) Superior</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+Buscamos uma Estagiária o para o Viveiro de Eucalipto da unidade de negócio Madeira da Florestal de Lençóis Paulista
+Se você tem atitude de dono acredita na liderança pelo exemplo e tem interesse em fazer parte de um ambiente colaborativo que fomenta a inovação e acredita na diversidade o seu ambiente é aqui na Dexco
+Inscrevase e venha fazer parte da nossa jornada de transformação
+Sobre a Florestal
+Desde o início de nossas atividades florestais fazemos questão de adotar práticas de manejo responsáveis que aliam altíssima produtividade à conservação da biodiversidade em todas as nossas unidades sendo inclusive considerados referência no setor
+Possuímos mais de 150 mil hectares de florestas de eucalipto e áreas de conservação que também servem de refúgio para mais de 24 mil espécies de fauna e flora</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Lençóis Paulista - SP</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://dexcogeracaod.gupy.io/job/eyJqb2JJZCI6Nzk5NTgxMywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Estágio - Operacional de Produtos</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Estágio - Operacional de Produtos</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DA VAGA
+Essa vaga é pra você se
+Tiver abertura para adquirir novos conhecimentos
+Tiver boa comunicação
+For uma pessoa proativa e resiliente
+Com capacidade de organização e execução</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Copiar link</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>São Paulo - SP</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://lidercap.gupy.io/job/eyJqb2JJZCI6Nzk5NzUyMCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat - relatorio com gemini + gráficos
</commit_message>
<xml_diff>
--- a/Vagas-Catho.xlsx
+++ b/Vagas-Catho.xlsx
@@ -471,32 +471,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vaga de Estágio em Pedagogia</t>
+          <t>Vaga de Estágio em Arquitetura e Urbanismo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FADELITO GLOBAL</t>
+          <t>SUPER ESTAGIOS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Auxiliar na elaboração de planos de aula Apoiar na execução de atividades pedagógica Acompanhar o desenvolvimento dos alunos Colaborar na organização de eventos educacionais Contribuir para a melhoria contínua dos processos educacionais</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Auxiliar nas seguintes atividades Acompanhamento de obras Suporte na Elaboração de projetos Experiência de campo Levantamento arquitetônico Projetos interiores Necessário Excel intermediário AutoCad e Reddit A partir do 7 período em um dos cursos Morar próximo a Jacarepaguá</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>200000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>São Paulo - SP (1)</t>
+          <t>Rio de Janeiro - RJ (1)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30447734/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-arquitetura-e-urbanismo/30692595/</t>
         </is>
       </c>
     </row>
@@ -516,25 +514,21 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Realizar atendimentos aos pacientes na recepção
-Realizar agendamentos via WhatsApp
-Auxiliar nas atividades administrativas da clínica
-Colaborar com a equipe multidisciplinar Boa comunicação</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Realizar lançamentos de pagamentos no sistema auxiliar na organização da Unidade agenda e manutenção de agendas de reuniões acompanhar prestadores de serviço fazer as cotações e compras de materiais de insumo da Unidade
+ Ter boa comunicação Ser proativo</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>200000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sorocaba - SP (1)</t>
+          <t>São Paulo - SP (1)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio/30702202/</t>
+          <t>https://www.catho.com.br/vagas/estagio/30731456/</t>
         </is>
       </c>
     </row>
@@ -544,38 +538,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vaga de Estágio</t>
+          <t>Vaga de Estágio Fonoaudiologia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>EMPRESA CONFIDENCIAL</t>
+          <t>CLÍNICA MENTHALHELP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Auxiliar na separação de peças conferencia dos pedidos etiquetar produtos organizar locação de peças 
- Cursando ensino superior em Engenharia Elétrica Mecânica ou áreas afins
-Conhecimento básico em componentes automotivos
-Boa comunicação e habilidades interpessoais
-Experiência prévia em estágios na área automotiv
-Conhecimento em sistemas de gestão
-Inglês intermediário</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t>O Fonoaudiólogo é responsável por avaliar pacientes com distúrbios de comunicação identificando problemas de fala linguagem voz audição e motricidade oral Desenvolvimento de planos de tratamento Com base na avaliação dos pacientes o Fonoaudiólogo desenvolve planos de tratamento personalizados com o objetivo de ajudar os pacientes a superar seus problemas de comunicação Realização de terapias O Fonoaudiólogo realiza terapias para ajudar os pacientes a desenvolver habilidades de comunicação corrigir problemas de fala linguagem voz audição e motricidade oral Acompanhamento e monitoramento O Fonoaudiólogo acompanha e monitora o progresso dos pacientes durante o tratamento realizando ajustes nos planos de tratamento quando necessário Orientação aos pacientes e familiares O Fonoaudiólogo orienta os pacientes e seus familiares sobre como melhorar a comunicação e prevenir futuros distúrbios Trabalho em equipe O Fonoaudiólogo trabalha em equipe com outros profissionais da saúde como médicos psicólogos e terapeutas ocupacionais para fornecer tratamento integrado aos pacientes Pesquisa e educação Alguns Fonoaudiólogos realizam pesquisas e participam de atividades de educação continuada para manterse atualizados sobre os avanços em sua área e melhorar suas habilidades profissionais O objetivo geral do trabalho do Fonoaudiólogo é melhorar a qualidade de vida dos pacientes ajudandoos a superar seus problemas de comunicação e melhorar sua autoestima e autoconfiança O trabalho do Fonoaudiólogo é importante em muitos contextos incluindo escolas hospitais clínicas e empresas onde pode ajudar a melhorar a comunicação e a produtividade das pessoas
+Ter fácil acesso a região de Guarulhos
+Deverá estar cursando Fonoaudiologia Estar cursando mínimo 4 semestre Estar cursando fonoaudiologia mínimo 4 semestre</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>200100300000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Caxias do Sul - RS (1)</t>
+          <t>Guarulhos - SP (2)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio/30703859/</t>
+          <t>https://www.catho.com.br/vagas/estagio-fonoaudiologia/30078566/</t>
         </is>
       </c>
     </row>
@@ -585,33 +573,36 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vaga de Estágio</t>
+          <t>Vaga de Estágio - Financeiro</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EMPRESA CONFIDENCIAL</t>
+          <t>ELIS ENERGIA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Recebimento de Mercadoria Conferência e Embalagem de Produtos Contagem cíclica de estoques Expedição de Pedidos Conferência de Nota Fiscal recebida Reposição de Estoques Separação de Pedidos Organizado responsável proativo ágil
-Requisitos técnicos Conhecimento World Excel</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t>1 Apoio na análise de dados financeiros e contábeis 
+2 Apoio no desenvolvimento de apresentações e memorandos
+3 Auxílio nas pesquisas de mercado e players 
+4 Auxílio na elaboração de modelos financeiros para avaliação de projetos e colaborações em teses de investimento e oportunidades de MA
+5 Apoio na elaboração de relatórios financeiros e contábeis Boa comunicação interpessoal e trabalho em equipe Crítico Senso de Dono Atitude proativa e capacidade de resolver problemas de forma eficaz Interesse em aprender sobre o contexto financeiro em empresa de energia solar
+Conhecimento Intermediário do Pacote Office Excel e PowerPoint Avançado 
+Inglês Intermediário será um diferencial</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>200000</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Caxias do Sul - RS (1)</t>
+          <t>São Paulo - SP (1)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio/30702704/</t>
+          <t>https://www.catho.com.br/vagas/estagio-financeiro/30730987/</t>
         </is>
       </c>
     </row>
@@ -621,41 +612,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Vaga de estágio</t>
+          <t>Vaga de Estágio em Direito</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LUIZ EDMUNDO MACHADO CORRETAGEM DE IMOVEIS</t>
+          <t>ADVOCACIA FELIZARDO BARROSO &amp; ASSOCIADOS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Auxiliar no atendimento aos clientes e na prospecção de novos negócios
-Realizar visitas a imóveis e apresentar as opções disponíveis
-Participar de reuniões e treinamentos para aprimorar conhecimentos
-Manter atualizado o sistema de cadastro de imóveis
-Auxiliar na elaboração de contratos de compra e venda
-Colaborar com a equipe em atividades administrativas Ensino Médio completo
-Conhecimento básico em informática
-Boa comunicação oral e escrita
-Experiência prévia em atendimento ao cliente
-Espirito empreendedor</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Acompanhamento de Processos Elaboração de Petições Distribuições Extração de Guias Cursando direito entre o 4 e 8 períodos</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>200000</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>São Paulo - SP (1)</t>
+          <t>Rio de Janeiro - RJ (1)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio/30681882/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-direito/30733545/</t>
         </is>
       </c>
     </row>
@@ -665,34 +645,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vaga de estágio</t>
+          <t>Vaga de Estágio de Marketing</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CLÍNICA LIFE FISIO SANTOS</t>
+          <t>EMPRESA CONFIDENCIAL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Acompanhar a Fisioterapeuta em sessões de fisioterapia ortopédica ou desportiva
-Aplicar Aula de Pilates junto com a fisioterapeuta
-Aplicar quando necessário liberação miofascial e drenagem linfática Curso de Pilates</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t xml:space="preserve"> Atuar no apoio às atividades de marketing 
+ Atuar no apoio aos eventos 
+ Atuar com demandas na organização de Podcast</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>200000</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Santos - SP (2)</t>
+          <t>Cuiaba - MT (1)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio/30675494/</t>
+          <t>https://www.catho.com.br/vagas/estagio-de-marketing/30731568/</t>
         </is>
       </c>
     </row>
@@ -702,38 +680,36 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Vaga de Estágio Direito</t>
+          <t>Vaga de Estágio de Enfermagem</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PERIM AUTO PEÇAS</t>
+          <t>COMERCIAL DAHANA LIMITADA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Elaboração de peça processual 1º e 2º grau
-Acompanhamento de processos
-Emissão de Guias
-Relatórios 
-Negociação Judicial e Extrajudicial
-Pesquisa Jurisprudencial
-Controle de Prazos</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Realizar avaliações de saúde ocupacional
+Realizar campanhas de saúde
+Realizar atendimento ambulatorial
+Realizar arquivo de documentos
+Documentar registros de saúde Deverá estar cursando Graduação em andamento no curso de enfermagem
+Disponibilidade para atuar em Contagem
+Disponibilidade para estagiar de 0800 às 1500</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>200000</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>São Paulo - SP (1)</t>
+          <t>Contagem - MG (1)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-direito/30701381/</t>
+          <t>https://www.catho.com.br/vagas/estagio-de-enfermagem/30731495/</t>
         </is>
       </c>
     </row>
@@ -743,32 +719,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Vaga de Estágio em Pedagogia</t>
+          <t>Vaga de Estágio em Administração</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AGIEER</t>
+          <t>ADVOCACIA FELIZARDO BARROSO &amp; ASSOCIADOS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ATIVIDADES Assistirá e acompanhará na recepção das criançasfamília e colher informações sobre a criança na entrada bem como repassar informações sobre a criança na saída auxiliar na análise e solicitar à família reposição de materiais de higiene pessoal da criança auxiliar no banho e troca das crianças e realizar os cuidados no despertar das crianças dar suporte ao lactário nas informações sobre a criança para a distribuição individual dos alimentos e bebidas ajudar no oferecimento à criança contribuir com informações para preenchimento de relatórios com as informações das crianças referentes a alimentação trocas de fralda sinais e sintomas elaborar registros de atividades participar de reuniões participar de treinamentos auxiliar na organização e do parque na confecção de materiais de eventos e brinquedos educativos auxiliar nos ensinamentos e nos cuidados e devoluções dos utensílios utilizados nas alimentações reposição de material de higiene e consumo organizar brinquedos pós higienização controlar e cuidas das trocas de roupas de cama REQUISITOS Residir na região da Lapa ou proximidades e estar cursando Pedagogia</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Atuar na área administrativa</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>200000</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>São Paulo - SP (1)</t>
+          <t>Rio de Janeiro - RJ (1)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30701138/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-administracao/30733464/</t>
         </is>
       </c>
     </row>
@@ -778,32 +752,31 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vaga de ESTÁGIO ADMINISTRATIVO</t>
+          <t>Vaga de Estágio na área Administrativa</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>OUTLET DA CONSTRUÇÃO LTDA</t>
+          <t>EMPRESA CONFIDENCIAL</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Auxiliar no cadastro de fornecedores e produtos Apoiar autorizando notas de compras no sistema Apoiar em lançamentos de notas fiscais Auxiliar no controle das notas faturadas no CNPJ da empresa Auxiliar na emissão de notas de devolução de fornecedores baixas e transferência de estoque e bonificações Auxiliar no controle de estoque dos produtos emissão de nota de baixaentrada dos mesmos A partir do 3º período CIÊNCIAS CONTÁBEIS Segunda a Sexta 08h as 12h e das 13h as 15h com 1h de almoço Valor da bolsa R100000 e vale transporte</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t xml:space="preserve"> Auxílio na distribuição de demandas de estagiários  Atualização de Planilhas de Controle de Qualidade  Auxílio no Tratamento de Dados em Planilhas do Google Sheets  Acompanhamento de Gestão de Estagiários sanando dúvidas de escala envio de atestados e outros  Revisão de textos
+  Boa Comunicação oral e escrita  Boa organização  Conhecimento linguístico gramatical e de norma culta  Se interessar por escrever e revisar texto</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>200000</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Lauro de Freitas - BA (1)</t>
+          <t>Campinas - SP (1)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-administrativo/30700649/</t>
+          <t>https://www.catho.com.br/vagas/estagio-na-area-administrativa/30731099/</t>
         </is>
       </c>
     </row>
@@ -813,43 +786,31 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Vaga de ESTÁGIO EM PEDAGOGIA</t>
+          <t>Vaga de Estagio em contabilidade</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>EMPRESA CONFIDENCIAL</t>
+          <t>HOMMAGE CONTABILIDADE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Seu currículo foi selecionado em nosso banco de dados para participar de um processo seletivo conforme condições abaixo
-Vaga Estágio Pedagogia
-Regime Contrato 6 meses
-Bolsa Auxílio R 85000
-Benefícios Vale transporte cesta básica possibilidade de prorrogação e possibilidade de efetivação
-Quantidade de vagas 2
-Horário do Estágio Das 1100 hs às 1700 hs
-Início Imediato
-Requisitos Pontualidade organização e atuação com qualidade e compromisso nos procedimentos estabelecidos no regimento escolar
-Nível Superior em Pedagogia  cursando 
-Horário de estudo A distância Noturno
-Atividades de estágio auxiliar no desenvolvimento de atividades pedagógicas prestar apoio na elaboração de projetos educacionais desenvolver atividades recreativas assessorar a professora nas rotinas de cuidados em sala de aula higiene alimenteção etc Até 4º Semestre</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Escrituração de notas fiscais de entrada e saída mercadorias e serviços geração de boletos do escritório e entregar em contato com os clientes para realizar cobranças fechando os recebíveis
+ Ser pró ativo ser responsável pelo trabalho cumprindo metas e prazos ter boa comunicação interna e externa</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>200000</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Ribeirão Pires - SP (2)</t>
+          <t>São Paulo - SP (1)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30054732/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-contabilidade/30732901/</t>
         </is>
       </c>
     </row>
@@ -859,36 +820,38 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Vaga de Estagio em Direito</t>
+          <t>Vaga de Estágio em Projetos</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ROCHA MARINHO E SALES ADVOGADOS</t>
+          <t>FERRARI SOLUÇÕES EM ENGENHARIA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Acompanhar audiências judiciais representando o escritório em casos de menor complexidade sob a supervisão de advogados
-Elaborar atas minutas de audiências e pareceres processuais
-Preparar e organizar documentos a serem utilizados nas audiências
-Realizar diligências externas junto aos fóruns e tribunais
-Prestar suporte aos advogados auxiliando na análise e no acompanhamento de processos</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Até R$ 2.000,00</t>
-        </is>
+          <t>Carga horária 4 horas  Período a combinar
+Auxiliar na elaboração de projetos das edificações com plantas cortes e fachadas medições e conferência de layout in loco
+Auxiliar na implantação do sistema de segurança contra incêndio em projetos memoriais de cálculos e documentos
+Auxiliar nas vistorias técnicas para adequações de imóveis no âmbito da segurança contra incêndio
+Auxiliar elaboração de orçamentos atendimento telefônico rotinas administrativas gerenciamento de compras e logística de materiais
+  Estagiário de curso arquiteturaengenhariatecnólogo partir do terceiro semestre Boa escrita e interpretação de textos e projetos
+Conhecimentos de projeto avançado em Auto CAD
+ Conhecimentos no pacote Office Word Outlook Excel desejável conhecimento em maquete 3D
+ Fácil acesso estamos localizados próximo a linha amarela estação Vila Sônia</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>200000</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Fortaleza - CE (1)</t>
+          <t>São Paulo - SP (1)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-direito/30702103/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-projetos/30733327/</t>
         </is>
       </c>
     </row>
@@ -898,32 +861,38 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Vaga de Estágio de Direito</t>
+          <t>Vaga de VAGA DE ESTÁGIO EM DIREITO</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>EMPRESA CONFIDENCIAL</t>
+          <t>IDEALIZA CIDADES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Protocolos Guias Organização de arquivos Petições diversas Andamento processual Atendimento ao cliente Perfil analítico Comprometimento Próatividade Organização Pontualidade Pacote office Excelente comunicação verbal e escrita Deve ter experiências em escritórios de advocacia Residir em CampinasSP</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t xml:space="preserve"> Elaboração de contratos
+ Pesquisa de jurisprudência
+ Análise de legislação 
+ Auxiliar na elaboração de pareceres jurídicos
+ Auxiliar no processo de registro de loteamentos e condomínios
+ Elaboração de documentos para registro de Associação de Moradores
+ Cursando 3º ano de Direito
+Disponibilidade de estágio presencial
+Interesse na área do Direito Imobiliário</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>200000</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Campinas - SP (1)</t>
+          <t>São Paulo - SP (1)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-de-direito/30700977/</t>
+          <t>https://www.catho.com.br/vagas/vaga-de-estagio-em-direito/30732830/</t>
         </is>
       </c>
     </row>
@@ -933,34 +902,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Vaga de Estágio em Administração</t>
+          <t>Vaga de VAGA DE ESTÁGIO EM DIREITO</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>SAMVARDHANA MOTHERSON REYDEL COMPANIES</t>
+          <t>IDEALIZA CIDADES</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>A Motherson Group é um fornecedor de soluções completas para a indústria automotiva global está entre os 21 maiores fornecedores com mais rápido crescimento atende a várias indústrias tais como material rodante aeroespacial médico TI e logística com mais de 135000 colaboradores mundialmente distribuídos em 42 países pelo mundo 
-Samvardhana Motherson Reydel Companies SMRC é a especialista do grupo em interiores inovadores de automóveis e caminhões Com instalações na Europa Ásia e América do Sul projetamos desenvolvemos e fabricamos sistemas internos completos de alta qualidade como cockpits consoles centrais painéis de portas e superfícies decorativas para várias montadoras de veículos em todo o mundo Em razão do nosso rápido crescimento estamos constantemente procurando novos e talentosos colegas para fazerem parte da nossa equipe
-Você está procurando uma oportunidade de crescimento e desenvolvimento na área de Administração
-A Motherson Group uma grande empresa do setor automotivo está com uma vaga de Estágio em Administração disponível
-Como estagiárioa de Administração você será responsável por
- Auxiliar nas atividades administrativas da empresa como controle de documentos arquivamento atendimento ao público e organização de rotinas
- Participar de projetos e atividades relacionadas à área de Administração como análise de processos elaboração de relatórios e suporte a tomada de decisões
- Aprender e adquirir novas habilidades aplicando os conhecimentos adquiridos durante sua formação acadêmica   Para se candidatar a esta vaga é necessário
- Estar cursando Administração ou áreas afins formação a partir de 2026
- Possuir habilidades de comunicação organização e trabalho em equipe
- Ter conhecimentos básicos em informática como pacote Office
- Ser proativoa comprometidoa e interessadoa em aprender</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t xml:space="preserve"> Elaboração de contratos
+ Pesquisa de jurisprudência
+ Análise de legislação 
+ Auxiliar na elaboração de pareceres jurídicos
+ Auxiliar no processo de registro de loteamentos e condomínios
+ Elaboração de documentos para registro de Associação de Moradores
+ Ï Cursando 3º ano de Direito
+Ï Disponibilidade de estágio presencial
+Ï Interesse na área do Direito Imobiliário</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>200000</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -969,7 +933,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-administracao/30701178/</t>
+          <t>https://www.catho.com.br/vagas/vaga-de-estagio-em-direito/30731462/</t>
         </is>
       </c>
     </row>
@@ -979,40 +943,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Vaga de Estágio em Nutrição</t>
+          <t>Vaga de Estágio Administrativo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>B&amp;P DESENVOLVIMENTO HUMANO</t>
+          <t>ELIS BRASIL</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Auxiliar na elaboração e controle de cardápios e fichas técnicas de produção considerando aspectos nutricionais e legislações vigentes
-  Acompanhar a implementação das boas práticas de manipulação de alimentos BPF e do controle de qualidade
-  Apoiar a equipe na verificação de validade e condições de armazenamento dos insumos alimentares
-  Colaborar na realização de treinamentos sobre higiene segurança alimentar e manipulação de alimentos para a equipe da padaria
-  Participar do controle de custos ajudando na gestão de desperdícios e na otimização de ingredientes
-  Monitorar o atendimento a requisitos de dietas especiais como opções sem glúten ou lactose
-  Auxiliar no desenvolvimento de novos produtos e receitas nutritivas para o portfólio da padaria
-   Cursando Técnico ou Superior em Nutrição
- </t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t>Atuará em atividades relacionadas a área administrativa e atendimento de clientes internos e externos Residir em Jundiaí e região</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Santo Andre - SP (1)</t>
+          <t>Jundiai - SP (1)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-nutricao/30701246/</t>
+          <t>https://www.catho.com.br/vagas/estagio-administrativo/30730722/</t>
         </is>
       </c>
     </row>
@@ -1022,32 +976,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Vaga de Estágio de Direito</t>
+          <t>Vaga de Estágio em Economia</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ROSSI ADVOCACIA</t>
+          <t>EMPRESA CONFIDENCIAL</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Guias Organização de arquivos Petições diversas Andamento processual Atendimento ao cliente protocolos Cursando Direito Perfil analítico Comprometimento Próatividade Organização Pontualidade Pacote office Excelente comunicação verbal e escrita Deve ter experiências em escritórios de advocacia Residir em CampinasSP</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t>conciliação e lançamento das operações dos fundos de investimento execução das rotinas operacionais dos sistemas contratados suporte na elaboração de relatórios diários e mensais de rentabilidade e risco das carteiras gerenciamento de caixa Excel</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Campinas - SP (1)</t>
+          <t>Diadema - SP (1)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-de-direito/30700940/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-economia/30732579/</t>
         </is>
       </c>
     </row>
@@ -1057,32 +1009,43 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Vaga de Estágio em Direito</t>
+          <t>Vaga de Estágio em Vendas</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OLÍMPIO DE AZEVEDO ADVOGADOS</t>
+          <t>EVOCONT CONTABILIDADE DIGITAL</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Estágio em Direito Interno  Auxiliar o Advogado em consulta processual aos principais sites do judiciário  Elaboração e conferência de guias de recolhimento de custas judiciais  Complementação de cadastros  Peticionamento simples em conjunto com o Advogado  Preenchimento de planilhas relatórios  Digitalização e arquivamento de documentos e correspondências jurídicas  Obtenção de cópias  Carga de processos  Despacho de petições com juízes Benefícios Seguro de Vida em Grupo Vale Transporte Regime de contratação Estágio Horário A combinar Deverá estar cursando Ensino Superior em Direito Pacote office básico Vontade de aprender</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
+          <t xml:space="preserve">Atividades
+Atuação junto a equipe comercial no atendimento de cliente em loja
+Auxiliar no controle de estoque físico e fluxo de caixa
+Auxiliar na geração de orçamentos e cadastro de clientes
+Auxiliar em pedidos para abastecimento de estoque
+Auxiliar na divulgação de campanhas nas redes sociais
+Auxiliar na organização geral do mostruário
+Habilidades
+Ótima comunicação proatividade e organização
+Requisitos
+Cursando Gestão Comercial Processos Gerenciais Administração Marketing e áreas correlatas
+Conhecimento intermediário do Pacote Office
+Jornada de Trabalho
+Segunda a sextafeira 0900h às 1500h </t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>São Paulo - SP (1)</t>
+          <t>Mogi-guaçu - SP (1)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.catho.com.br/vagas/estagio-em-direito/30701062/</t>
+          <t>https://www.catho.com.br/vagas/estagio-em-vendas/30732770/</t>
         </is>
       </c>
     </row>
@@ -1092,33 +1055,34 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4016474 : Programa de Estágio TIM RJ</t>
+          <t>Estágio administrativo - Contas a receber</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4016474 : Programa de Estágio TIM RJ</t>
+          <t>Estágio administrativo - Contas a receber</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-SomosMaisNaTIM Fazer parte da TIM é se conectar com o que acreditamos e ter MAIS sintonia com todo o TIMe É aprender novas formas de oferecer ao mundo um trabalho com MAIS propósito Aprendizado na TIM é MAIS que possibilidade É o que nos move a fazer MAIS e melhor É desenvolver habilidades com criatividade e transformar tecnologia em MAIS liberdade Tecnologia na TIM é MAIS que ter a melhor cobertura É imaginar as possibilidades com MAIS inovação conectando todos e todas com respeito e agilidade Diversidade e Inclusão na TIM é MAIS que abraçar É uma cultura cada vez MAIS essencial para o nosso dia a dia É criar um impacto MAIS positivo sendo quem você é Vem ser você e fazer parte de um TIMe que tem a coragem para inovar a liberdade para tentar e a vontade de fazer a diferença na vida das pessoas imagineaspossibilidades</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+Você quer fazer parte da maior especialista em tecnologia da América Latina Com um portfólio que reúne mais de 10000 fabricantes e mais de 1000000 de títulos em software estamos presentes no Brasil México e Colômbia com um alcance que se estende por toda a América
+Se você é apaixonado por tecnologia e busca constante aprendizado queremos você em nosso time
+Venha trilhar uma jornada de crescimento e desenvolvimento profissional que fará a diferença na sua carreira
+Inscrevase agora e ajude a vamos juntos construir o futuro da tecnologia</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://programastim.gupy.io/job/eyJqb2JJZCI6Nzk5ODg0OCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://software.gupy.io/job/eyJqb2JJZCI6ODAxNTEwNiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1128,33 +1092,38 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4013980 : Programa de Estágio TIM RJ</t>
+          <t>Estágio em Engenharia Civil</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>4013980 : Programa de Estágio TIM RJ</t>
+          <t>Estágio em Engenharia Civil</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-SomosMaisNaTIM Fazer parte da TIM é se conectar com o que acreditamos e ter MAIS sintonia com todo o TIMe É aprender novas formas de oferecer ao mundo um trabalho com MAIS propósito Aprendizado na TIM é MAIS que possibilidade É o que nos move a fazer MAIS e melhor É desenvolver habilidades com criatividade e transformar tecnologia em MAIS liberdade Tecnologia na TIM é MAIS que ter a melhor cobertura É imaginar as possibilidades com MAIS inovação conectando todos e todas com respeito e agilidade Diversidade e Inclusão na TIM é MAIS que abraçar É uma cultura cada vez MAIS essencial para o nosso dia a dia É criar um impacto MAIS positivo sendo quem você é Vem ser você e fazer parte de um TIMe que tem a coragem para inovar a liberdade para tentar e a vontade de fazer a diferença na vida das pessoas imagineaspossibilidades</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+Antes de falarmos sobre a vaga que tal entender um pouco sobre nós
+Somos uma construtora pura focada em empreendimentos de médio e alto padrão na região metropolitana de São Paulo Temos como propósito desenvolver espaços onde as pessoas sejam acolhidas com dignidade prazer e se sintam melhores onde moram trabalham se hospedam consomem e investem
+São mais de 40 obras concluídas Em nosso portifólio temos obras residenciais comerciais hotéis e saúde
+Nossos pilares de negócios são a excelência a sustentabilidade e a inovação
+Valorizamos nossos talentos por isso mais de 40 do nosso time é formado dentro de casa Estamos crescendo muito e claro queremos que nosso time cresça com a gente
+Ajudar a construir o futuro de São Paulo não é somente criar projetos é também gerar valor pra sociedade através da solidariedade de projetos sustentáveis parcerias duradouras e respeito ao meio ambiente Buscamos quem partilha destes princípios e acredita ser possível transformar o futuro de São Paulo
+Criamos um ambiente familiar e profissional de integração que proporcione a coletividade de reconhecimento mútuo estimulamos que seja colaborativo e positivo Aqui todas as pessoas são bem vindas e respeitadas em suas diferentes origens crenças experiências raças deficiências orientações sexuais e gerações
+VEMPRAROCONTEC</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://programastim.gupy.io/job/eyJqb2JJZCI6Nzk5ODgwMCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://rocontec.gupy.io/job/eyJqb2JJZCI6ODAxMTA2Mywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1164,27 +1133,29 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PROGRAMA DE ESTÁGIO 2025 - FARMÁCIA</t>
+          <t>Estagio em Engenharia Civil - Obra</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PROGRAMA DE ESTÁGIO 2025 - FARMÁCIA</t>
+          <t>Estagio em Engenharia Civil - Obra</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-Estão abertas as inscrições para o Programa de Estágio em Farmácia 2025 do Hospital Alemão Oswaldo Cruz
-Venha fazer parte de um time que é referência no País responsável por colaborar e destacar o Oswaldo Cruz como um dos melhores centros hospitalares da América Latina
-O Hospital é composto por pessoas que têm compromisso com o paciente e foco em qualidade e segurança Somos orientados para o resultado e por isso temos uma atuação inovadora e liderança inspiradora Estamos há 126 anos promovendo o cuidado inclusive de quem cuida
-Trazemos de nossa origem alemã algumas características como o respeito pelo outro a valorização do coletivo a verdade a discrição e a austeridade E isso se reflete ao que todos os colaboradores se propõem a cada dia Immer Besser  Fazer sempre melhor</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+Antes de falarmos sobre a vaga que tal entender um pouco sobre nós
+Somos uma construtora pura focada em empreendimentos de médio e alto padrão na região metropolitana de São Paulo Temos como propósito desenvolver espaços onde as pessoas sejam acolhidas com dignidade prazer e se sintam melhores onde moram trabalham se hospedam consomem e investem
+São mais de 40 obras concluídas Em nosso portifólio temos obras residenciais comerciais hotéis e saúde
+Nossos pilares de negócios são a excelência a sustentabilidade e a inovação
+Valorizamos nossos talentos por isso mais de 40 do nosso time é formado dentro de casa Estamos crescendo muito e claro queremos que nosso time cresça com a gente
+Ajudar a construir o futuro de São Paulo não é somente criar projetos é também gerar valor pra sociedade através da solidariedade de projetos sustentáveis parcerias duradouras e respeito ao meio ambiente Buscamos quem partilha destes princípios e acredita ser possível transformar o futuro de São Paulo
+Criamos um ambiente familiar e profissional de integração que proporcione a coletividade de reconhecimento mútuo estimulamos que seja colaborativo e positivo Aqui todas as pessoas são bem vindas e respeitadas em suas diferentes origens crenças experiências raças deficiências orientações sexuais e gerações
+VEMPRAROCONTEC</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1193,7 +1164,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://hospitaloswaldocruz.gupy.io/job/eyJqb2JJZCI6Nzk5ODI5MSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://rocontec.gupy.io/job/eyJqb2JJZCI6Nzk1NTE1MSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1203,33 +1174,38 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4045902 : Programa de Estágio TIM RJ</t>
+          <t>Programa de Estágio - Futuros Líderes Maxpar</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4045902 : Programa de Estágio TIM RJ</t>
+          <t>Programa de Estágio - Futuros Líderes Maxpar</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-SomosMaisNaTIM Fazer parte da TIM é se conectar com o que acreditamos e ter MAIS sintonia com todo o TIMe É aprender novas formas de oferecer ao mundo um trabalho com MAIS propósito Aprendizado na TIM é MAIS que possibilidade É o que nos move a fazer MAIS e melhor É desenvolver habilidades com criatividade e transformar tecnologia em MAIS liberdade Tecnologia na TIM é MAIS que ter a melhor cobertura É imaginar as possibilidades com MAIS inovação conectando todos e todas com respeito e agilidade Diversidade e Inclusão na TIM é MAIS que abraçar É uma cultura cada vez MAIS essencial para o nosso dia a dia É criar um impacto MAIS positivo sendo quem você é Vem ser você e fazer parte de um TIMe que tem a coragem para inovar a liberdade para tentar e a vontade de fazer a diferença na vida das pessoas imagineaspossibilidades</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+          <t xml:space="preserve">DESCRIÇÃO DA VAGA
+Olá D
+ Já pensou em fazer parte de um Grupo Brasileiro com mais de 6000 colaboradores e ter a oportunidade conhecer diferentes áreas além de ser capacitado a e desafiado a e se tornar um futuro líder de equipe
+ Estamos em busca de talentos que se identifiquem com uma carreira de liderança que tenham sede de aprendizado e queiram fazer a diferença O programa Futuros Líderes tem duração de 6 meses a 1 ano e o objetivo vai muito além da efetivação de um contrato de estágio queremos formar líderes para crescer com a gente
+ Você terá a oportunidade de atuar e conhecer diversos setores relacionados ao Negócio Maxpar e receber suporte e mentoria de gestores que são referência fornecendo um processo de desenvolvimento contínuo e enriquecedor
+ Se você é apaixonadoa por inovação pensa fora da caixa trazendo soluções busca um ambiente de ebulição de ideias gosta de trabalhar em equipe deseja desenvolvimento contínuo e plano de carreira seu lugar é aqui Inscrevase hoje 
+ FuturosLíderesMaxpar
+OrgulhoDeSerGrupoAutoglass
+ </t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>Vila Velha - ES</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://programastim.gupy.io/job/eyJqb2JJZCI6Nzk5NzIzNiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://autoglassestagio.gupy.io/job/eyJqb2JJZCI6ODAxNDUyMiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1239,35 +1215,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Estágio Jurídico</t>
+          <t>Pessoa Estagiária de Atendimento</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Estágio Jurídico</t>
+          <t>Pessoa Estagiária de Atendimento</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO DA VAGA
-Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais arbitrais e extrajudiciais
-Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias pareceres opiniões legais desenvolvimento de negócios elaboração e estruturação de contratos
-O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito seja no âmbito regional nacional ou internacional São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+          <t xml:space="preserve">DESCRIÇÃO DA VAGA
+A SiMCo foi criada com o foco em oferecer atendimento médico e odontológico de qualidade aos 150 milhões de brasileiros que não possuem planos de saúde privados SiM significa Serviço de Inclusão à Medicina e a cor verde sinaliza para as pessoas sinal verde para um serviço de saúde acessível de alta qualidade
+Vem com a gente construir a maior e melhor plataforma de acesso à saúde da América Latina </t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Campo Grande - MS</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6Nzk5ODE5NSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://simco.gupy.io/job/eyJqb2JJZCI6Nzk4OTE4Niwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1277,35 +1250,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Estágio Jurídico</t>
+          <t>Estágio - Trading de Energia</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Estágio Jurídico</t>
+          <t>Estágio - Trading de Energia</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais arbitrais e extrajudiciais
-Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias pareceres opiniões legais desenvolvimento de negócios elaboração e estruturação de contratos
-O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito seja no âmbito regional nacional ou internacional São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+Nossa cliente é uma empresa pioneira no Brasil autorizada a comercializar energia elétrica com consumidores finais e geradores no ambiente de contratação livre
+Área Comercialização de Energia</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Campo Grande - MS</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6Nzk5ODE4Nywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://vagascetefe.gupy.io/job/eyJqb2JJZCI6ODAwNDk3Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1315,35 +1285,33 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Estágio Jurídico</t>
+          <t>Estágio - Atendimento</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Estágio Jurídico</t>
+          <t>Estágio - Atendimento</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais arbitrais e extrajudiciais
-Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias pareceres opiniões legais desenvolvimento de negócios elaboração e estruturação de contratos
-O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito seja no âmbito regional nacional ou internacional São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+Buscamos uma pessoa para atuar como estagiário de atendimento na MRM Brasil uma agência fullservice com maior foco em digital do McCann Worldgroup unidade do Grupo Interpublic IPG Uma agência que acredita no poder das intersecções entre estratégia criatividade e tecnologia suportado por dados para criar experiências totalmente humanas Atuamos a partir do modelo híbrido de agência e consultoria de transformação digital ajudando a fortalecer o relacionamento entre negócios e pessoas ajudando marcas a encontrarem seu propósito aprofundar suas relações e criar experiências que gerem crescimento
+ A MRM Brasil valoriza a criatividade e inovação algo que é potencializado em um ambiente diverso e inclusivo por isso damos prioridade na contratação de grupos minoritários como pessoas com mais de 45 anos pretas pardas indígenas pessoas da comunidade LGBTQIAP e PCDs
+ Venha fazer parte de um time Better Together onde sua individualidade é respeitada e valorizada em todos os sentidos</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Campo Grande - MS</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6Nzk5ODE4Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://mrm.gupy.io/job/eyJqb2JJZCI6ODAxMzIyNSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1353,38 +1321,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Estagiária(o) Superior</t>
+          <t>Estágio em Segurança do Trabalho</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Estagiária(o) Superior</t>
+          <t>Estágio em Segurança do Trabalho</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-Buscamos uma Estagiária o para o Viveiro de Eucalipto da unidade de negócio Madeira da Florestal de Lençóis Paulista
-Se você tem atitude de dono acredita na liderança pelo exemplo e tem interesse em fazer parte de um ambiente colaborativo que fomenta a inovação e acredita na diversidade o seu ambiente é aqui na Dexco
-Inscrevase e venha fazer parte da nossa jornada de transformação
-Sobre a Florestal
-Desde o início de nossas atividades florestais fazemos questão de adotar práticas de manejo responsáveis que aliam altíssima produtividade à conservação da biodiversidade em todas as nossas unidades sendo inclusive considerados referência no setor
-Possuímos mais de 150 mil hectares de florestas de eucalipto e áreas de conservação que também servem de refúgio para mais de 24 mil espécies de fauna e flora</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+A Krones do Brasil Ltda está em busca de um profissional motivado que almeje se desenvolver profissionalmente e queira crescer dentro da empresa para fazer parte da nossa equipe de Segurança do Trabalho O profissional executará atividades para eliminação de riscos e prevenção de acidentes na organização visando proteger e resguardar a integridade dos empregados próprios e terceiros bem como apoiará os de Meio Ambiente e Qualidade
+SolutionsBeyondTomorrow BePartOfKrones</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Lençóis Paulista - SP</t>
+          <t>Diadema - SP</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://dexcogeracaod.gupy.io/job/eyJqb2JJZCI6Nzk5NTgxMywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://krones.gupy.io/job/eyJqb2JJZCI6ODAxNDEzMSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>
@@ -1394,28 +1356,26 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Estágio - Operacional de Produtos</t>
+          <t>Estágio de Social Media</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Estágio - Operacional de Produtos</t>
+          <t>Estágio de Social Media</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>DESCRIÇÃO DA VAGA
-Essa vaga é pra você se
-Tiver abertura para adquirir novos conhecimentos
-Tiver boa comunicação
-For uma pessoa proativa e resiliente
-Com capacidade de organização e execução</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Copiar link</t>
-        </is>
+Se você se identifica com uma gestão horizontal com menos burocracia e mais ação e valoriza a autonomia para trazer e concretizar ideias evoluindo e crescendo no processo venha fazer parte do nosso time de uniques
+Estamos em busca de uma pessoa para atuar como estagiária de Social Media na Briefing
+A Briefing é nossa agência de DJs e bandas com a missão de identificar as necessidades de diferentes tipos de clientes e oferecer o artista mais adequado
+A vaga é presencial de segunda a quinta com home office às sextas no período da manhã ou tarde
+A empresa está localizada no Jardim Paulista próxima ao Parque Ibirapuera e à Avenida Juscelino Kubitschek</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1424,7 +1384,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://lidercap.gupy.io/job/eyJqb2JJZCI6Nzk5NzUyMCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+          <t>https://umauma.gupy.io/job/eyJqb2JJZCI6ODAxMzcxMywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat - selector not find
</commit_message>
<xml_diff>
--- a/Vagas-Catho.xlsx
+++ b/Vagas-Catho.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
   <si>
     <t>nome</t>
   </si>
@@ -34,450 +34,371 @@
     <t>link vaga</t>
   </si>
   <si>
-    <t>Vaga de Estágio em Engenharia Civil - Obras</t>
-  </si>
-  <si>
-    <t>Vaga de Estagio</t>
-  </si>
-  <si>
-    <t>Vaga de ESTAGIO</t>
+    <t>Vaga de ESTAGIO PEDAGOGIA - COTIA</t>
   </si>
   <si>
     <t>Vaga de Estágio</t>
   </si>
   <si>
-    <t>Vaga de ESTÁGIO DE ARQUITETURA</t>
+    <t>Vaga de ESTÁGIO</t>
+  </si>
+  <si>
+    <t>Vaga de estagio</t>
+  </si>
+  <si>
+    <t>Vaga de Estágio em Engenharia</t>
+  </si>
+  <si>
+    <t>Vaga de Estágio em Direito</t>
+  </si>
+  <si>
+    <t>Vaga de Estagio em Marketing</t>
+  </si>
+  <si>
+    <t>Vaga de Estágio Administrativo</t>
+  </si>
+  <si>
+    <t>Vaga de ESTAGIO DP</t>
   </si>
   <si>
     <t>Vaga de Estágio em Administração</t>
   </si>
   <si>
-    <t>Vaga de Estágio em Marketing</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio em Design</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio em Contabilidade</t>
-  </si>
-  <si>
-    <t>Vaga de estágio em e-commerce</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio em Vendas</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio - Contábil</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio Administrativo</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio de Engenharia</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio em Logística</t>
-  </si>
-  <si>
-    <t>Vaga de Estágio em Edificações</t>
-  </si>
-  <si>
-    <t>Estágio em Processos de Customer Success</t>
-  </si>
-  <si>
-    <t>ESTÁGIO - BACKOFFICE CONTA CORRENTE</t>
-  </si>
-  <si>
-    <t>Estágio em Estratégia e M&amp;A</t>
-  </si>
-  <si>
-    <t>Estágio em Biblioteconomia</t>
-  </si>
-  <si>
-    <t>Estágio - Núcleo de Negociação (período 13:00 - 18:00)</t>
-  </si>
-  <si>
-    <t>Estágio de Pedagogia | Zona Leste</t>
-  </si>
-  <si>
-    <t>ESTÁGIO ADMINISTRATIVO NA CORRETORA DE SEGUROS</t>
+    <t>Vaga de Estágio em Letras</t>
+  </si>
+  <si>
+    <t>Vaga de Estágio em Jornalismo</t>
+  </si>
+  <si>
+    <t>Vaga de Estágio de Marketing</t>
+  </si>
+  <si>
+    <t>Vaga de Estágio em Pedagogia</t>
+  </si>
+  <si>
+    <t>Vaga de Estagio Administrativo</t>
+  </si>
+  <si>
+    <t>Vaga de ESTAGIO EM LOGÍSTICA</t>
   </si>
   <si>
     <t>Estágio Jurídico</t>
   </si>
   <si>
-    <t>Estágio Engenharia Mecânica</t>
+    <t>Estágio - Consignação</t>
+  </si>
+  <si>
+    <t>Estágio em Contabilidade | Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Estágio - Radiologia (CDI 24 DE OUTUBRO)</t>
+  </si>
+  <si>
+    <t>Vagas Estágio - Estagiário de Eventos</t>
+  </si>
+  <si>
+    <t>Pessoa Estagiária de Atendimento</t>
+  </si>
+  <si>
+    <t>Estágio em Operações | Caucaia</t>
+  </si>
+  <si>
+    <t>Programa de Estágio CSN | São Paulo/SP - Corporativo</t>
+  </si>
+  <si>
+    <t>FADELITO GLOBAL</t>
+  </si>
+  <si>
+    <t>KADU CABRAL ARQUITETURA</t>
+  </si>
+  <si>
+    <t>********</t>
+  </si>
+  <si>
+    <t>VENTURA INFORMATICA</t>
+  </si>
+  <si>
+    <t>GRUPO GPS</t>
   </si>
   <si>
     <t>EMPRESA CONFIDENCIAL</t>
   </si>
   <si>
-    <t>GUIMARÃES &amp; ROSSI ADVOGADOS</t>
-  </si>
-  <si>
-    <t>********</t>
-  </si>
-  <si>
-    <t>ESPAÇO CRIATIVO</t>
-  </si>
-  <si>
-    <t>JP PROJETOS</t>
-  </si>
-  <si>
-    <t>ESPACO CONVIVER E APRENDER</t>
-  </si>
-  <si>
-    <t>ONLINE EDITORA</t>
-  </si>
-  <si>
-    <t>GRUPO REAL RH EM PARCERIA COM EMPRESA ABRE 1 VAGA DE ESTÁGIO EM CONTABILIDADE.</t>
-  </si>
-  <si>
-    <t>CASSOL CENTERLAR</t>
-  </si>
-  <si>
-    <t>UNITRADING LOG</t>
-  </si>
-  <si>
-    <t>LOJA DO SAPO</t>
-  </si>
-  <si>
-    <t>ELECTRIC MOBILITY BRASIL</t>
-  </si>
-  <si>
-    <t>INSTALAR ENGENHARIA</t>
-  </si>
-  <si>
-    <t>"Acompanhar do dia a dia da obra, Manter a documentação em dia, Controlar a agenda de entregas, Acompanhar empreiteiros, Análise e execução de proposta técnica; Acompanhamento de obras e desenvolvimento de relatórios e planilhas. Preenchimento de planilhas e relatórios diária. Solicitação de compras e cotação. "Conhecimento básico em AutoCAD; Pacote Office; Profissional organizado, com iniciativa e facilidade de aprendizado.</t>
-  </si>
-  <si>
-    <t>Estabelecimento sem classificação</t>
-  </si>
-  <si>
-    <t>Venda do produto Consignado FGTS, utilizando a plataforma whatsapp. Ter entre 16 a 21 anos;
-Horário 7:00 as 14:00 (1 hora de almoço)
-Saber se comunicar com o cliente;
-Saber utilizar computador;
-Ter bom relacionamento com os colegas de trabalho;
-ter disponibilidade aos sábados( trabalho esporádico);
-disposição para aprender.</t>
-  </si>
-  <si>
-    <t>Realizar lançamentos de pagamentos no sistema; auxiliar na organização da Unidade, agenda e manutenção de agendas de reuniões; acompanhar prestadores de serviço, fazer as cotações e compras de materiais de insumo da Unidade.
- Ter boa comunicação, Ser proativo.</t>
-  </si>
-  <si>
-    <t>AUXÍLIO NA ELABORAÇÃO DE PROJETOS EM 3D, PROJETOS TÉCNICOS PARA APROVAÇÃO EM ÓRGÃOS PÚBLICOS, ACOMPANHAMENTO EM OBRAS COM AS ARQUITETAS. CONHECIMENTO NÍVEL MÉDIO A AVANÇADO EM AUTO CAD, CONHECIMENTO NÍVEL MÉDIO EM SKETCHUP E VRAY (RENDERIZADOR). NECESSÁRIO ENVIO DE PORTFÓLIO NO E-MAIL</t>
-  </si>
-  <si>
-    <t>Atuar no controle de custos administrativos;
-Realizar emissão e controle de registros técnicos;
-Ajudar na criação de relatórios e outros documentos administrativos;
-Colaborar na gestão de processos de compras e estoque;
-Auxiliar no controle e manutenção das unidades;
-Realizar envio, entrega e conferência de correios e plataformas de entrega;
-Auxiliar na organização de contratos e atualização de planilhas;
-Participar do desenvolvimento e implementação de procedimentos internos. Pacote office intermediário;
-Habilidades para cotação e negociação com parceiros e fornecedores;</t>
-  </si>
-  <si>
-    <t>Criação de conteúdo visual (fotos e vídeos) para nossas redes sociais
-Auxílio na produção de criativos, utilizando ferramentas como Canva
-Edição de vídeos simples com softwares como Inshot ou CapCut
-Apoio nas estratégias de marketing digital e mídias sociais
- Conhecimento básico em Canva
-Experiência com editores simples de vídeo (Inshot ou CapCut)
-Fácil acesso a Artur Alvim ZL</t>
-  </si>
-  <si>
-    <t>Auxiliar na criação de layouts, diagramação/ajustes de materiais; Auxilio no fechamento e montagem das matérias para serem impressas na gráfica; Auxilio na vetorização de ilustrações..
- Conhecimento nas seguintes ferramentas: Pacote Adobe (InDesign, Illustrator, Photoshop); Pacote Office. 
-Ser ágil, organizado e criativo. Capacidade de trabalhar com detalhes e prazos.</t>
-  </si>
-  <si>
-    <t>Classificação de lançamentos contábeis,
-Conciliação contábil;
-Emissão de relatórios contábeis;
-Inclusão de dados em sistema. Cursando Ciências Contábeis;
-Ter conhecimento intermediário no Pacote Office.</t>
-  </si>
-  <si>
-    <t>" Atualizar o site da empresa; 
-" Trabalhar na parte operacional das promoções; 
-" Acompanhar relatorios; 
-" Operar em outras atribuições administrativas. 
-Habilidade em análise de dados
-Proatividade e iniciativa
-Excel básico</t>
-  </si>
-  <si>
-    <t>Atenção estudantes Superior ou Técnico dos cursos Administração, Ciências contábeis, Gestão Comercial, Vendas, que residem no SUL DA ILHA.
-VAGA DE ESTÁGIO EM VENDAS
-Seu desafio será:
- Auxiliar no atendimento ao público;
-Auxiliar a manter o ambiente organizado;
-Auxiliar nas vendas e rotina. Administração, Ciências contábeis, Gestão Comercial, Vendas;</t>
-  </si>
-  <si>
-    <t>Auxiliar no processo de validação fiscal das notas fiscais de entrada;
-Auxiliar no processo de contas a pagar;
-Emitir de notas fiscais pertinente a operação;
-Preencher relatórios;
-Caso atenda as demandas pertinentes, possibilidade de efetivação.
- Cursando Ensino Superior em Ciências Contábeis
-Excel Básico</t>
-  </si>
-  <si>
-    <t>Atenção estudantes Técnico ou Superior em Administração, Gestão Comercial, Comércio Internacional, Recursos Humanos.
-VAGA ESTÁGIO ADMINISTRATIVO (HOME OFFICE)
-Seu desafio será:
--Suporte em registro e lançamento de dados nos sistemas e planilhas.
--Comunicação com clientes internos e externos;
--Auxiliar na cotação de viagens, reserva de eventos e hospedagens;
--Apoio nas atividades de administração. Técnico ou Superior em Administração, Gestão Comercial, Comércio Internacional, Recursos Humanos.</t>
-  </si>
-  <si>
-    <t>A Loja do Sapo é uma empresa focada na felicidade do nosso time!!!
-Somos uma Assistência Técnica Especializada em reparos nos produtos da marca apple (apple watch, ipad, Mac e Iphone) reparos como troca de vidro, touch, bateria, placa e pequenos componentes. Nossa Missão é reconectar as pessoas ao mundo digital com agilidade e excelência proporcionando alívio e entusiasmo em ter seu aparelho novo de novo. 
-Nosso grande sonho e visão é continuar sendo a maior empresa especializada de dispositivos Apple de Minas Gerais, e ser referência nacional em nosso segmento entregando solução ágil e encantadora aos nossos cientes.
-Aqui você encontra uma Cultura Forte que se destaca por promover um clima muito descontraído, leve, agradável e humano. Somos apaixonados pelos nossos valores de Encantamento, Inovação, Compromisso, Resultado, Adaptabilidade, Gratidão e Respeito. 
-Prezamos muito pela transparência, validando esse nosso zelo através dos nossos ritos internos de comunicação e alinhamento de expectativas. 
-Você encontra aqui também muita oportunidade de desenvolvimento através de treinamentos corriqueiros para o time, feedback para auxiliar o seu crescimento e muita parceria para alcançarmos o sucesso juntos! 
-Queremos aqui pessoas que além de compartilhar dos nossos valores, sejam profissionais dispostos a enfrentar desafios e propor melhorias para nossa evolução contínua, que tenham a visão do _x001C_Copo Cheio_x001D_, tenham aquela alegria no coração e força de vontade para fazer a diferença e entregar o algo a mais.
-Se identificou?! Convidamos você a ser um Starfrog!!!!
-Para a vaga de Estagiário de Engenharia buscamos um profissional que será responsável por analisar os processos existentes na empresa, avaliar junto as lideranças sua assertividade e propor melhorias de acordo com os dados analisados e implementar as melhorias na empresa. 
-Dia a Dia
-" Trabalhar no auxílio à gestão direta de gerentes e diretores da empresa 
-" Criação e manutenção de indicadores de gestão 
-" Desenvolvimento de relatórios para a tomada de decisão 
-" Auxílio no mapeamento e melhoria de processos 
-" Participação na execução de projetos chaves da empresa
-" Desenvolvimento de soluções (software)
-Requisitos e qualificações 
-" Graduação de Engenharia em andamento a partir do 4° período;
-" Excel Avançado
-" Interesse em programação (Python é diferencial);
-" Boa capacidade analítica
-" Proativo, Criativo e Inconformado.
-" Bom em trabalho em equipe e ávido por aprendizado e melhoria.
-O que você vai encontrar na Loja do Sapo: 
-- Bolsa estágio: R$ 1.600,00 
-- Cultura Incrível: Faça parte de uma atmosfera leve e agradável, promovendo um ambiente de trabalho inspirador.
-- Parcerias Exclusivas: Desfrute de momentos de lazer com acesso a piscinas, hospedagens e atividades diversas através da nossa parceria com o Sesc.
-- Benefícios Flexíveis: Escolha entre o Vale Transporte ou Auxílio Combustível, adaptando-se às suas necessidades.
-- Benefícios Exclusivos: Aproveite descontos em mais de 30 mil parceiros através do aplicativo Clube Certo e desfrute de um Day Off em seu aniversário para recarregar suas energias.
-- Flexibilidade Financeira: aproveite descontos exclusivos em produtos e serviços da nossa loja.
-Quer adquirir conhecimento na sua carreira? Vem para a #LojadoSapo</t>
-  </si>
-  <si>
-    <t>Recebimento e envio de mercadorias, cotação e escolha de transportes, análise e homologação de fornecedores de logística, implementação de fluxos, controle e gestão de estoque, agendamento e acompanhamento de coletas.
- Desejável conhecimento em Excel, sistemas de Gestão de Transporte e Inglês</t>
-  </si>
-  <si>
-    <t>Apoiar a equipe de projetistas e engenheiros na criação e revisão de projetos técnicos.
--Colaborar na análise de desenhos e especificações técnicas.
--Auxiliar na preparação de documentos e relatórios de projetos.
--Contribuir para a solução de problemas técnicos e otimização de processos. Ter habilidade no Revit ou AutoCad</t>
+    <t>ADONAI RH</t>
+  </si>
+  <si>
+    <t>LIGUE IMOVEIS</t>
+  </si>
+  <si>
+    <t>ORGANIZACAO CONTABIL LUIZA CANDIDO</t>
+  </si>
+  <si>
+    <t>não encontrado</t>
+  </si>
+  <si>
+    <t>COLÉGIO RAÍZES</t>
+  </si>
+  <si>
+    <t>KRONE CAPITAL</t>
+  </si>
+  <si>
+    <t>Irá auxiliar a titular de sala em todas as atividades pertinentes ao cuidados e atividades das crianças
+estar cursando pedagogia do primeiro ao penultimo semestre
+Deverá estar cursando: estar cursando pedagogia do primeiro ao penúltimo semestre Inicio imediato, gostar de atuar com crianças e contribuir com o desenvolvimento das delas em sala de aula.</t>
+  </si>
+  <si>
+    <t>Vaga destinada à desenvolvimento de projeto técnico, consistindo no detalhamento de projeto legal e executivo. O candidato ideal deve ter domínio em Revit e será um diferencial ter conhecimento em SketchUp e Enscape. O foco do nosso seguimento é Arquitetura comercial, com maior abrangência em restaurantes. Estudante de arquitetura a partir do 4º período e com cursos correlacionados, apresentando currículo, projetos de faculdade sobre projetos ou podendo apresentar até mesmo portfólio se houver.</t>
+  </si>
+  <si>
+    <t>AUXILIAR NA ELABORAÇÃO DE DESENHOS TÉCNICOS; AUXILIAR NA ELABORAÇÃO DE DOCUMENTOS, RELATÓRIOS E PLANILHAS; ACOMPANHAR ANÁLISES DE PROJETOS. SETOR DE PROJETOS ESTRUTURAIS E RODOVIÁRIOS Conhecimento em Autocad e Excel.</t>
+  </si>
+  <si>
+    <t>Elaboração de planilhas, cotação de produtos, e de frete, captação de cliente, emissão de nota, contas a pagar a receber, cadastro ao cliente ao fornecedor, cadastro de produtos. Conhecimento sobre o estoque.
+conhecimento em trabalho em plataforma, e-mail, zap ser produtivo, pontual, responsável, ambos sexo
+não ter vícios.
+idade 18 a 26 anos
+ter conhecimento World e excel</t>
+  </si>
+  <si>
+    <t>- Apoiar na elaboração do cronograma de manutenção preventiva.
+- Participar na criação de planos de manutenção com base nas orientações dos engenheiros e técnicos.
+Auxiliar na análise de histórico de manutenção para otimizar a periodicidade de inspeções e intervenções.
+- Acompanhar a abertura, execução e fechamento das Ordens de Serviço planejadas no sistema de gestão de manutenção (CMMS).
+- Verificar o status das OS abertas e auxiliar no controle de pendências.
+- Auxiliar na coleta e análise de indicadores como MTBF (Mean Time Between Failures), MTTR (Mean Time to Repair), e disponibilidade de equipamentos.
+- Participar no planejamento e execução de paradas programadas dos equipamentos industriais para manutenção.
+- Acompanhar a alocação de recursos (equipe, materiais e ferramentas) para garantir que o cronograma seja seguido. Cursando Ensino Superior em Engenharia Mecânica, Elétrica, Automação ou correlatas com previsão de formação em Dez'27
+Inglês em nível intermediário
+Diferenciais: Pacote Office, Sharepoint, Power BI, Power Apps e Power Automate</t>
+  </si>
+  <si>
+    <t>Acompanhamento de Processos, Elaboração de Petições, Distribuições, Extração de Guias. Cursando direito entre o 4° e 8° períodos.</t>
+  </si>
+  <si>
+    <t>auxiliar os demais profissionais na elaboração de um bom planejamento, informando estratégias que contribuam para o alcance dos objetivos e metas traçadas. Cursando o ensino superior</t>
+  </si>
+  <si>
+    <t>Dar suporte administrativo e operacional às demais áreas da empresa, com o atendimento telefônico e presencial, organização de arquivos, envio de documentos, recepção de clientes. Ser organizado(a), pois lidará com documentos internos da empresa. Saber trabalhar em equipe, uma vez que irá interagir com diversas áreas da empresa. Ter boa comunicação oral e escrita, devido às atividades exercidas.</t>
+  </si>
+  <si>
+    <t>Toda rotina do departamento pessoal Cursando RECURSOS HUMANOS - A PARTIR DO 3º SEMESTRE</t>
+  </si>
+  <si>
+    <t>Atuar na área administrativa.</t>
+  </si>
+  <si>
+    <t>Objetivo da Vaga: O estagiário em Letras tem como objetivo apoiar as atividades e projetos da área de Produção, focando em roteiros e conteúdos em texto e áudio, além de atuar em processos e projetos audiovisuais de acordo com suas demandas. O pensamento analítico, uso de metodologias ágeis e desenvolvimento profissional também farão parte do seu plano de desenvolvimento. Realizar locução ao vivo, respeitando padrões linguísticos; Decupagem de legenda; Realizar Audiodescrição e produção de roteiros dentro da plataforma; Revisão de texto; Apoiar time de produção com demais atividades relacionadas ao desenvolvimento de textos e locução. Atividades: 1. Realizar decupagem, dividindo o roteiro por cena e planejamento; 2. Fazer a edição e correção de legendas; 3. Realizar Audiodescrição e produção de roteiros dentro da plataforma; 4. Controle de qualidade dos conteúdos produzidos; 5. Apoiar time de produção com demais atividades relacionadas ao desenvolvimento de textos e locução. Boa comunicação, habilidade em oratória e escrita;
+DIFERENCIAL: Pacote Google Office (não é requisito obrigatório/de desclassificação);
+DIFERENCIAL: idiomas inglês e/ou espanhol.</t>
+  </si>
+  <si>
+    <t>Objetivo da Vaga:
+O estagiário em Jornalismo tem como objetivo apoiar as atividades e projetos da área de Produção, focando em roteiros e conteúdos em texto e áudio, além de atuar em processos e projetos audiovisuais de acordo com suas demandas. O pensamento analítico, uso de metodologias ágeis e desenvolvimento profissional também farão parte do seu plano de desenvolvimento. Realizar locução ao vivo, respeitando padrões linguísticos; Decupagem de legenda; Realizar Audiodescrição e produção de roteiros dentro da plataforma;
+Revisão de texto; Apoiar time de produção com demais atividades relacionadas ao desenvolvimento de textos e locução. Atividades: 1. Realizar decupagem, dividindo o roteiro por cena e planejamento;
+2. Fazer a edição e correção de legendas; 3. Realizar Audiodescrição e produção de roteiros dentro da plataforma; 4. Controle de qualidade dos conteúdos produzidos; 5. Apoiar time de produção com demais atividades relacionadas ao desenvolvimento de textos e locução. Boa comunicação, habilidade em oratória e escrita;
+DIFERENCIAL: Pacote Google Office (não é requisito obrigatório/de desclassificação);
+DIFERENCIAL: idiomas inglês e/ou espanhol.</t>
+  </si>
+  <si>
+    <t>" Apoiar na criação de conteúdos para redes sociais, blogs e campanhas publicitárias, conforme orientação da equipe.
+" Monitorar e auxiliar na gestão das redes sociais da empresa, interagindo com o público e respondendo a comentários e mensagens.
+" Auxiliar na coleta e análise de dados de campanhas de marketing, como engajamento, taxa de conversão e alcance.
+" Contribuir para a pesquisa de mercado, analisando tendências e concorrentes, e apresentar relatórios para a equipe.
+" Ajudar na organização e suporte em eventos, promoções e ações de marketing.
+" Apoiar a equipe na criação e atualização de materiais promocionais, catálogos e informativos.
+" Participar de reuniões e colaborar com diferentes equipes para garantir a execução das estratégias de marketing.
+" Conhecimento básico em ferramentas de redes sociais e de design gráfico é um diferencial (Photoshop, Canva).
+" Familiaridade com plataformas de marketing digital e análise de dados será considerado um diferencial.
+" Certificações (Opcional):
+Certificações em marketing digital, como Google Digital Garage, HubSpot, ou similares, são consideradas um diferencial.</t>
+  </si>
+  <si>
+    <t>Irá acompanhar os alunos para atividdades a fins de recreação e alimentação. Está cursando o 2ºsemestre.</t>
+  </si>
+  <si>
+    <t>Emitir propostas comerciais e acompanhar seu progresso até a implantação.
+Resolver pendências nos processos administrativos, garantindo conformidade.
+Manter e atualizar o banco de dados com informações precisas e atualizadas.
+Planilhar e atualizar informações críticas para o setor.
+Pós-venda
+Fornecer atendimento ao cliente com serviço de concierge, incluindo agendamentos e fornecimento de informações.
+Realizar movimentações cadastrais, como inclusão e exclusão de funcionários.
+Oferecer suporte ao cliente, solucionando demandas específicas e gerenciando chamados com o SAC ou ANS. Domínio intermediário ou avançado do Pacote Office (Excel, Word, PowerPoint).
+Excelente comunicação verbal e escrita, com foco em um atendimento atencioso e esclarecedor.
+Alta capacidade de organização, atenção a detalhes e habilidade para resolver problemas de forma autônoma.
+Desejável experiência anterior em funções administrativas ou de atendimento ao cliente.</t>
+  </si>
+  <si>
+    <t>ESTÁGIO EM LOGÍSTICA
+- Cursando 2º módulo do curso em Logística
+- Conhecimento em Excel e informática
+PARA RIBEIRÃO PIRES</t>
   </si>
   <si>
     <t>DESCRIÇÃO DA VAGA
-Estamos em busca de um(a) estagiário(a) proativo(a) e cheio(a) de energia para integrar nossa equipe de Customer Success, atuando diretamente em atividades administrativas e de processos. Se você gosta de desafios, é analítico(a), organizado(a) e quer crescer em um ambiente dinâmico e colaborativo, essa é a sua chance de fazer a diferença!
-Está em nosso DNA inovar sem medo de errar. Aqui, nós aprendemos, desaprendemos e reaprendemos a todo instante. Ser flexível e pensar com ousadia e foco em resultados é o nosso lema! Estamos sempre buscando gente que tem o olhar aberto ao mundo e a todas as possibilidades que ele oferece, gente que não tem medo de se reinventar diante dos desafios. Se você tem comprometimento com o que faz e adora descomplicar, o seu lugar pode ser aqui! #VemSerBern ✨</t>
+Há setenta anos o escritório Ernesto Borges Advogados presta serviços jurídicos para a resolução de conflitos judiciais, arbitrais e extrajudiciais.
+Com significativo espólio de experiências multidisciplinares o escritório atende os interesses de seus clientes na definição de estratégias, pareceres, opiniões legais, desenvolvimento de negócios, elaboração e estruturação de contratos.
+O escritório se destaca nas mais abrangentes áreas de especialidades e setores econômicos e se destaca na conquista de prêmios e reconhecimentos em diversas áreas do direito, seja no âmbito regional, nacional ou internacional. São conquistas importantes obtidas por consequência do propósito de prestar serviços jurídicos de excelência, aplicado com eficiência pelas lideranças e desenvolvido com persistência por todos os profissionais que compõem o time do Ernesto Borges Advogados.</t>
   </si>
   <si>
     <t>DESCRIÇÃO DA VAGA
-#VEMSERMERCANTIL
-Ei, você! Ser desafiado diariamente é algo que te motiva? Se a resposta for sim, vem ser Mercantil! O que não faltam aqui são oportunidades de estágio para vivenciar novos desafios e ser protagonista de sua carreira, tudo isso em uma das Melhores Empresas para se trabalhar em Minas Gerais. 
-E essa combinação fica ainda mais perfeita se você tiver brilho nos olhos, uma comunicação sensacional, proatividade e, claro, foco em resultados. Curtiu? Então, veja abaixo a oportunidade que temos aqui:
-O QUE VOCÊ PRECISA TER
-Estudantes de ensino superior, devidamente matriculados na instituição de ensino;
-Disponibilidade para cumprir 2 anos do Programa de Estágio;
-Disponibilidade para estagiar durante o período de 06 horas (manhã).
-Cursos: Administração, Ciências Contábeis, Controladoria e Finanças
-VOCÊ SE DESTACA COM
-Pacote Office: Word, Excel, Power Point
- COMO VOCÊ VAI ATUAR AQUI
-Auxílio na análise de documentos de clientes para abertura de contas;
-Apoio no cadastro e na atualização de dados cadastrais de pessoas físicas e jurídicas;
-Auxílio no atendimento de demandas internas e preenchimento de planilhas;
-Apoio na manutenção de dados em aplicativos relativos às atividades descritas acima.
- O QUE OFERECEMOS
-Bolsa de R$2.236,24 e após 90 dias R$2.449,58;
-Vale transporte - sem desconto no valor da bolsa;
-Gympass e Programa Meu Bem-Estar;
-Sua saúde é muito importante para nós. Com esse convênio, você terá acesso a centenas de serviços para se cuidar: da vida fitness até yoga!
-Seguro de vida - sem desconto no valor da bolsa;
-Academia Mercantil de Desenvolvimento
-Pra você se preparar e ser cada vez mais protagonista da sua carreira, em nossa parceria com a Uol e milhares de cursos.
-Todas as vagas também são direcionadas para PCDs.</t>
+A Livraria da Vila tem como objetivo proporcionar uma boa experiência para o cliente.
+Simpatia, acolhimento, disponibilidade e muita leitura fazem parte do nosso jeito de ser.
+Se você gosta de livros e de interagir com pessoas, seu lugar é aqui!
+ Para a vaga de estágio buscamos candidatos com perfil analítico, organizado, que goste de processos e rotinas administrativas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIÇÃO DA VAGA
+A Supergasbras é uma empresa do grupo holandês SHV Energy, líder mundial na distribuição de Gás liquefeito de Petróleo (GLP), com mais de 100 anos de experiência. Nosso negócio é levar energia limpa e eficiente para milhões de brasileiros, seja nas suas casas, comércios, indústrias ou agronegócio. Os mais de 76 anos de atuação no Brasil nos posiciona como uma das principais distribuidoras nacionais de GLP - comercializamos cerca de 1,5 milhão de toneladas do produto por ano com aproximadamente 20% de participação de mercado.
+Desenvolvemos uma série de projetos com foco em transformação digital, experiência do cliente, inovação e desenvolvimento sustentável do negócio. Nossa estratégia é conseguir através da confiança e integridade, ser a melhor empresa de Energia do Brasil para nossos clientes, parceiros, colaboradores e acionistas, com responsabilidade socioambiental.
+Diversidade e inclusão é uma prioridade de negócios para a Supergasbras. Valorizamos e acreditamos no desenvolvimento de pessoas, tanto no contexto profissional como pessoal, tendo como estratégia a equidade de gênero, inclusão de pessoas com deficiência, respeito a todas as orientações sexuais e luta contra a discriminação racial nas diferentes camadas da sociedade.
+Ser diverso é ser Super!  </t>
   </si>
   <si>
     <t>DESCRIÇÃO DA VAGA
-Somos uma das maiores empresas de geração e comercialização de energia 100% renovável do país, com um portfólio de 745 MW e um pipeline de projetos para dobrar a nossa capacidade nos próximos anos. Levamos a sério a nossa estratégia de ESG e zelamos pelo nosso bom ambiente de trabalho onde as pessoas colaboram e se sentem seguras para serem elas mesmas, se desenvolver e entregar resultados.
-Você que é da área de Administração, Economia Contábeis ou Engenharias, quer desenvolver ainda mais a sua carreira ao lado de um time de alta performance, em um ambiente dinâmico e com exposição a alta liderança da empresa?
-Se você respondeu sim e está a fim de novos desafios, está esperando o que para fazer parte do nosso time de Estratégia e M&amp;A?</t>
+Atuar na área de Centro de Diagnóstico da Unimed (CDU), acompanhando exames radiológicos; auxiliando no posicionamento do paciente para realização do exame; higienizando equipamentos de imagem sob a supervisão do técnico em radiologia.</t>
   </si>
   <si>
     <t>DESCRIÇÃO DA VAGA
-Há 26 anos, somos movidos por um único objetivo: transformar vidas por meio da educação. A Escola do Futuro prepara o aluno para o mundo. Somos uma escola multicultural, cristã e bilíngue, acreditamos que esses são desenvolvimentos necessários para o mundo que vivemos hoje, tornando dessa forma o aluno preparado muito mais do que a se comunicar com o mundo inteiro, mas também transformá-lo num lugar melhor.
-Estudante do 3º ano de Biblioteconomia, Letras, Jornalismo ou História, em busca de uma oportunidade para aplicar seus conhecimentos teóricos em situações práticas do ambiente profissional
-Junte-se ao nosso Time!</t>
+Com mais de 30 anos de presença no setor bancário de atacado, somos uma instituição financeira comprometida com a excelência e inovação. Estamos atravessando um momento de grandes transformações comprometidos com o crescimento estratégico e investindo em um novo modelo operacional, colocando a centralidade no cliente como nossa prioridade máxima. para sustentar nosso crescimento estratégico e manter a satisfação dos clientes.
+Nossa trajetória é marcada por inovação, integridade e um compromisso inabalável com a excelência. Estamos empenhados em proporcionar um ambiente de trabalho dinâmico, onde a criatividade e a liderança são incentivadas.
+Junte-se a uma organização que valoriza a criatividade e o pensamento inovador e participe ativamente de uma fase transformadora que irá contribuir para o seu próprio crescimento profissional. Incentivamos a aprendizagem contínua em um ambiente colaborativo e fornecemos recursos para o desenvolvimento de habilidades.</t>
   </si>
   <si>
     <t>DESCRIÇÃO DA VAGA
-Estamos à procura de estudantes engajados, com boa argumentação e persuasão.
-Estes estagiários serão responsáveis pelo auxilio na negociação e recuperação de créditos (cobrança).
-Se você é comunicativo e movido a desafios, essa é uma oportunidade incrível para se juntar ao nosso time.</t>
+A SiMCo foi criada com o foco em oferecer atendimento médico e odontológico de qualidade aos 150 milhões de brasileiros que não possuem planos de saúde privados. SiM significa Serviço de Inclusão à Medicina e a cor verde sinaliza para as pessoas sinal verde para um serviço de saúde acessível de alta qualidade.
+Vem com a gente construir a maior e melhor plataforma de acesso à saúde da América Latina! 🚀💚💜</t>
   </si>
   <si>
     <t>DESCRIÇÃO DA VAGA
-Buscamos um (a) Estagiário (a) de Pedagogia para nos ajudar a transformar a educação do Brasil.
-Conheça mais sobre a gente:
-A Rede Decisão é a rede de escolas com maior visão de expansão do país, buscamos oferecer um ensino de qualidade a um preço acessível. Priorizamos a excelência pedagógica por meio de uma metodologia eficaz, pessoas dedicadas e uma rotina de estudos estruturada para os nossos estudantes. 
-Uma rede de escolas com mais de 30 anos no mercado, buscando o melhor para o seu futuro, respeitando a diversidade e cultivando um ambiente com altas expectativas onde todos são protagonistas e responsáveis.
-Hoje já somos um time de 1.400 colaboradores, 650 professores e 11.200 alunos espalhados por São Paulo, Campinas e Minas Gerais. 
-E aí, curtiu? Venha fazer parte da Rede Decisão!
-#VemPraRede</t>
-  </si>
-  <si>
-    <t>DESCRIÇÃO DA VAGA
-Estamos buscando uma Pessoa Estagiária, para atuar no time da ImobSeguros;
-Sua missão e desafios será fornecer apoio administrativo crucial para garantir a eficiente gestão de clientes da corretora de seguros. Fará a interacao com seguradoras e parceiros para esclarecimento de duvidas e envio de documentos.
-Se você tem uma visão inovadora, ama desafios e quer crescer em um ambiente colaborativo, o seu lugar é aqui! ❤️</t>
-  </si>
-  <si>
-    <t>DESCRIÇÃO DA VAGA
-Com o compromisso de contribuir para o progresso econômico e tecnológico, o bem-estar social e o desenvolvimento sustentável dos mercados em que atuamos, queremos contar a sua ENERGIA, para nos ajudar a CONSTRUIR a nossa trajetória como empresa líder nos segmentos que operamos.</t>
-  </si>
-  <si>
-    <t>DESCRIÇÃO DA VAGA
-O programa de Estágio da Brascabos tem como foco principal desenvolver o seu talento, ainda em formação, auxiliando no seu desenvolvimento profissional e transformando o conhecimento teórico em aplicações práticas.
-Desafio: Identificar, melhorar, inovar e automatizar equipamentos, dispositivos, processos produtivos, de qualidade e logístico.
-Então ...
-#VemSerBrascabos</t>
+JUNTE-SE À CSN!
+A Companhia Siderúrgica Nacional busca atrair e desenvolver profissionais que se identifiquem com a sua cultura, valorizando sempre a diversidade. Venha você também fazer parte da história do maior complexo siderúrgico da América Latina, um grupo que tem como essência “fazer bem, fazer mais e fazer para sempre”.
+O Programa de Estágio CSN é ideal para quem busca uma oportunidade de ingressar no mundo corporativo em um ambiente que estimula, desenvolve e potencializa.
+Já imaginou iniciar a sua carreira no maior complexo siderúrgico integrado da América Latina? #VEMSERCSN!
+Se você é estudante dos cursos de Ciências Contábeis, Recursos Humanos, Administração, Ciências Econômicas, Gestão Financeira, Engenharias, Matemática, Estatística, Psicologia, Comunicação, Tecnologia da Informação, ou áreas correlatas, com previsão de conclusão entre Junho/2026 e dezembro/2026, este programa é para você!</t>
+  </si>
+  <si>
+    <t>Cotia - SP (1)</t>
+  </si>
+  <si>
+    <t>Manaus - AM (2)</t>
+  </si>
+  <si>
+    <t>Londrina - PR (2)</t>
+  </si>
+  <si>
+    <t>Vila Velha - ES (1)</t>
+  </si>
+  <si>
+    <t>Indaiatuba - SP (1)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro - RJ (1)</t>
   </si>
   <si>
     <t>São Paulo - SP (1)</t>
   </si>
   <si>
-    <t>Belo Horizonte - MG (1)</t>
-  </si>
-  <si>
-    <t>Bragança Paulista - SP (5)</t>
-  </si>
-  <si>
-    <t>Guarulhos - SP (3)</t>
-  </si>
-  <si>
-    <t>Barueri - SP (2)</t>
-  </si>
-  <si>
-    <t>Campinas - SP (1)</t>
-  </si>
-  <si>
-    <t>São Jose - SC (1)</t>
-  </si>
-  <si>
-    <t>Florianópolis - SC (1)</t>
+    <t>Caxias do Sul - RS (1)</t>
   </si>
   <si>
     <t>Barueri - SP (1)</t>
   </si>
   <si>
-    <t>Estágio</t>
-  </si>
-  <si>
-    <t>Belo Horizonte - MG</t>
+    <t>Aparecida de Goiania - GO (1)</t>
+  </si>
+  <si>
+    <t>Ribeirão Pires - SP (1)</t>
+  </si>
+  <si>
+    <t>Campo Grande - MS</t>
   </si>
   <si>
     <t>São Paulo - SP</t>
   </si>
   <si>
-    <t>Ribeirão Preto - SP</t>
-  </si>
-  <si>
-    <t>Florianópolis - SC</t>
-  </si>
-  <si>
     <t>Rio de Janeiro - RJ</t>
   </si>
   <si>
-    <t>Rio Claro - SP</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-engenharia-civil-obras/30131317/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio/30749238/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio/30737421/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio/30731456/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-de-arquitetura/30748634/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-administracao/30749248/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-marketing/30749373/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-design/30749718/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-contabilidade/30749145/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-e-commerce/30749053/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-vendas/30748789/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-contabil/30749041/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-administrativo/30749432/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-de-engenharia/30738137/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-logistica/30742078/</t>
-  </si>
-  <si>
-    <t>https://www.catho.com.br/vagas/estagio-em-edificacoes/30741608/</t>
-  </si>
-  <si>
-    <t>https://vemserbern.gupy.io/job/eyJqb2JJZCI6ODAwNTA5Nywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://estagiomercantil.gupy.io/job/eyJqb2JJZCI6ODAyNTcxMiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://ibitu.gupy.io/job/eyJqb2JJZCI6ODAyNTQ3Miwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://escoladofuturo.gupy.io/job/eyJqb2JJZCI6ODAyNTM0MCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://ramosbenedettiadvogados.gupy.io/job/eyJqb2JJZCI6ODAxNjYyOSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://vemprarededecisao.gupy.io/job/eyJqb2JJZCI6ODAyNDk2MSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://imobseguros.gupy.io/job/eyJqb2JJZCI6ODAyNDg3OSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://sejaelecnordobrasil.gupy.io/job/eyJqb2JJZCI6Nzk5NDkxNSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
-  </si>
-  <si>
-    <t>https://vemserbrascabos.gupy.io/job/eyJqb2JJZCI6NzkxMjYyMywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+    <t>Porto Alegre - RS</t>
+  </si>
+  <si>
+    <t>Fortaleza - CE</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-pedagogia-cotia/30741822/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio/30798557/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio/30772872/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio/30772247/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-engenharia/30799368/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-direito/30798697/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-marketing/30798448/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-administrativo/30797676/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-dp/30797474/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-administracao/30798722/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-letras/30798851/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-jornalismo/30798375/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-de-marketing/30797583/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-pedagogia/30798409/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-administrativo/30797951/</t>
+  </si>
+  <si>
+    <t>https://www.catho.com.br/vagas/estagio-em-logistica/30797742/</t>
+  </si>
+  <si>
+    <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6ODA2Mjg1NSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://ernestoborges.gupy.io/job/eyJqb2JJZCI6ODA2Mjg1MCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://livrariadavila.gupy.io/job/eyJqb2JJZCI6ODA2MjQyNywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://supergasbras.gupy.io/job/eyJqb2JJZCI6ODA2MjQyMywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://unimedpoa.gupy.io/job/eyJqb2JJZCI6Nzk1NzUyNiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://abcbrasil.gupy.io/job/eyJqb2JJZCI6Nzk4MTkzMCwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://simco.gupy.io/job/eyJqb2JJZCI6ODAxMjA1Mywic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://supergasbras.gupy.io/job/eyJqb2JJZCI6ODA2MjAzNiwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
+  </si>
+  <si>
+    <t>https://csn.gupy.io/job/eyJqb2JJZCI6ODA2MTk2OSwic291cmNlIjoiZ3VweV9wb3J0YWwifQ==?jobBoardSource=gupy_portal</t>
   </si>
 </sst>
 </file>
@@ -882,19 +803,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -905,19 +826,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -928,19 +849,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>200000</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -951,19 +872,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>200000</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -977,16 +898,16 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>200000</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1000,16 +921,16 @@
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>200000</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1023,16 +944,16 @@
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>200000</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1046,16 +967,16 @@
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>200000</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1069,16 +990,16 @@
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10">
         <v>200000</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1089,19 +1010,19 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>200000</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1112,19 +1033,19 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1135,19 +1056,19 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1158,19 +1079,19 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1181,19 +1102,19 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15">
         <v>200000</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1204,19 +1125,19 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16">
         <v>200000</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1227,19 +1148,19 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1253,16 +1174,16 @@
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1270,22 +1191,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1293,22 +1214,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1316,22 +1237,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1339,22 +1260,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1362,22 +1283,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1385,22 +1306,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1408,22 +1329,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1431,22 +1352,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>